<commit_message>
updated buffer dist, new demo results
</commit_message>
<xml_diff>
--- a/demo_results.xlsx
+++ b/demo_results.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/serrislew/Desktop/CMU/18-500 Capstone/AutonomousDrivingModels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C33A0BAE-CD3E-B642-A97B-65710804D901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECE3973-FF07-4E42-BBFE-846C8C88DAB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="scale = 25" sheetId="1" r:id="rId1"/>
-    <sheet name="scale = 20" sheetId="4" r:id="rId2"/>
+    <sheet name="25" sheetId="5" r:id="rId1"/>
+    <sheet name="20" sheetId="6" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="results" localSheetId="1">'scale = 20'!$A$1:$L$7</definedName>
+    <definedName name="results" localSheetId="1">'20'!$A$1:$L$7</definedName>
+    <definedName name="results" localSheetId="0">'25'!$A$1:$L$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,8 +35,26 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="results" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{4C0F06DF-E766-9A4C-9845-1D2A7DCA8CE9}" name="results1" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/serrislew/Desktop/CMU/18-500 Capstone/AutonomousDrivingModels/results.csv" comma="1">
+      <textFields count="12">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" xr16:uid="{244D4666-79CD-4D46-B62F-C8FAEBFD2305}" name="results2" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="10000" sourceFile="/Users/serrislew/Desktop/CMU/18-500 Capstone/AutonomousDrivingModels/results.csv" comma="1">
       <textFields count="12">
         <textField/>
@@ -98,7 +117,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -637,7 +656,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results" connectionId="1" xr16:uid="{1BE21446-64E6-4547-BEA8-04CC74B54DD9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results" connectionId="2" xr16:uid="{EB18F3DE-7027-0F4E-B08C-0E21543D17EE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -936,318 +959,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30DB464B-5D17-F342-B5A9-DB655657D429}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6.5" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="5" width="23" customWidth="1"/>
-    <col min="6" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" customWidth="1"/>
-    <col min="9" max="9" width="27.1640625" customWidth="1"/>
-    <col min="10" max="10" width="29" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" customWidth="1"/>
-    <col min="12" max="13" width="18.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>20</v>
-      </c>
-      <c r="B2">
-        <v>33</v>
-      </c>
-      <c r="C2">
-        <v>0.96704245161699998</v>
-      </c>
-      <c r="D2">
-        <v>7.3665745482E-3</v>
-      </c>
-      <c r="E2">
-        <v>5.83276441073E-2</v>
-      </c>
-      <c r="F2">
-        <v>2.69347423977</v>
-      </c>
-      <c r="G2">
-        <v>26</v>
-      </c>
-      <c r="H2">
-        <v>0.76027337140399998</v>
-      </c>
-      <c r="I2">
-        <v>2.6879666786200001E-2</v>
-      </c>
-      <c r="J2">
-        <v>8.3160659982099996E-2</v>
-      </c>
-      <c r="K2">
-        <v>4.2269002596499998</v>
-      </c>
-      <c r="L2">
-        <v>26.923076923099998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>33</v>
-      </c>
-      <c r="C3">
-        <v>1.0698377791</v>
-      </c>
-      <c r="D3">
-        <v>5.6567676106799997E-3</v>
-      </c>
-      <c r="E3">
-        <v>2.4654766578E-2</v>
-      </c>
-      <c r="F3">
-        <v>1.3239212334199999</v>
-      </c>
-      <c r="G3">
-        <v>26</v>
-      </c>
-      <c r="H3">
-        <v>0.84315900182199999</v>
-      </c>
-      <c r="I3">
-        <v>1.9787714687699999E-2</v>
-      </c>
-      <c r="J3">
-        <v>7.5982566771599994E-2</v>
-      </c>
-      <c r="K3">
-        <v>3.6716403663200001</v>
-      </c>
-      <c r="L3">
-        <v>26.923076923099998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>21</v>
-      </c>
-      <c r="C4">
-        <v>0.43235468338799998</v>
-      </c>
-      <c r="D4">
-        <v>8.7882283087999998E-3</v>
-      </c>
-      <c r="E4">
-        <v>8.3873406284000002E-2</v>
-      </c>
-      <c r="F4">
-        <v>10.6349020371</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>2.5162032046799999E-2</v>
-      </c>
-      <c r="I4">
-        <v>1.27198541797E-3</v>
-      </c>
-      <c r="J4">
-        <v>8.6057231518800001E-2</v>
-      </c>
-      <c r="K4">
-        <v>19.185340056099999</v>
-      </c>
-      <c r="L4">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>20</v>
-      </c>
-      <c r="B5">
-        <v>33</v>
-      </c>
-      <c r="C5">
-        <v>0.759589897046</v>
-      </c>
-      <c r="D5">
-        <v>1.48969614641E-2</v>
-      </c>
-      <c r="E5">
-        <v>9.7624172486600005E-2</v>
-      </c>
-      <c r="F5">
-        <v>5.0454444289199998</v>
-      </c>
-      <c r="G5">
-        <v>25</v>
-      </c>
-      <c r="H5">
-        <v>0.56918323372299995</v>
-      </c>
-      <c r="I5">
-        <v>2.8904113956699999E-2</v>
-      </c>
-      <c r="J5">
-        <v>9.1344068984499996E-2</v>
-      </c>
-      <c r="K5">
-        <v>5.7606441775999997</v>
-      </c>
-      <c r="L5">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>20</v>
-      </c>
-      <c r="B6">
-        <v>34</v>
-      </c>
-      <c r="C6">
-        <v>0.94236709428200005</v>
-      </c>
-      <c r="D6">
-        <v>7.47914985275E-3</v>
-      </c>
-      <c r="E6">
-        <v>8.0821440428899993E-2</v>
-      </c>
-      <c r="F6">
-        <v>3.3123255968100001</v>
-      </c>
-      <c r="G6">
-        <v>25</v>
-      </c>
-      <c r="H6">
-        <v>0.70732558429500003</v>
-      </c>
-      <c r="I6">
-        <v>2.77793581256E-2</v>
-      </c>
-      <c r="J6">
-        <v>8.6239632272400002E-2</v>
-      </c>
-      <c r="K6">
-        <v>4.800710392</v>
-      </c>
-      <c r="L6">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>20</v>
-      </c>
-      <c r="B7">
-        <v>33</v>
-      </c>
-      <c r="C7">
-        <v>0.75655779235200005</v>
-      </c>
-      <c r="D7">
-        <v>1.0274405866500001E-2</v>
-      </c>
-      <c r="E7">
-        <v>7.8132675866999998E-2</v>
-      </c>
-      <c r="F7">
-        <v>5.2497121492999996</v>
-      </c>
-      <c r="G7">
-        <v>25</v>
-      </c>
-      <c r="H7">
-        <v>0.56994449006000003</v>
-      </c>
-      <c r="I7">
-        <v>2.7561351267899999E-2</v>
-      </c>
-      <c r="J7">
-        <v>9.4566862959499995E-2</v>
-      </c>
-      <c r="K7">
-        <v>5.7846301595399998</v>
-      </c>
-      <c r="L7">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B8">
-        <f>SUM(B2:B7)</f>
-        <v>187</v>
-      </c>
-      <c r="G8">
-        <f>SUM(G2:G7)</f>
-        <v>128</v>
-      </c>
-      <c r="L8">
-        <f>(B8-G8)*100/G8</f>
-        <v>46.09375</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1309,37 +1025,37 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C2">
-        <v>0.874659201379</v>
+        <v>0.983637105186</v>
       </c>
       <c r="D2">
-        <v>3.67807367918E-3</v>
+        <v>6.3752976485100003E-3</v>
       </c>
       <c r="E2">
-        <v>1.52008494326E-2</v>
+        <v>6.18717058257E-2</v>
       </c>
       <c r="F2">
-        <v>0.95742225647000001</v>
+        <v>2.4790107939000001</v>
       </c>
       <c r="G2">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H2">
-        <v>0.71445774592800004</v>
+        <v>0.79590500144499998</v>
       </c>
       <c r="I2">
-        <v>1.15210979619E-2</v>
+        <v>1.7345520589300001E-2</v>
       </c>
       <c r="J2">
-        <v>5.1493304656200001E-2</v>
+        <v>7.2813992217499998E-2</v>
       </c>
       <c r="K2">
-        <v>3.2168751557699999</v>
+        <v>3.5153008302100002</v>
       </c>
       <c r="L2">
-        <v>25</v>
+        <v>22.222222222199999</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1347,37 +1063,37 @@
         <v>20</v>
       </c>
       <c r="B3">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C3">
-        <v>0.89478802919900002</v>
+        <v>0.69806578918899997</v>
       </c>
       <c r="D3">
-        <v>1.9946184918799999E-3</v>
+        <v>1.25092295428E-2</v>
       </c>
       <c r="E3">
-        <v>9.5692874686100007E-3</v>
+        <v>0.125113840591</v>
       </c>
       <c r="F3">
-        <v>0.85953697562200004</v>
+        <v>5.9225344841299998</v>
       </c>
       <c r="G3">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H3">
-        <v>0.80001510537499998</v>
+        <v>0.45899929867</v>
       </c>
       <c r="I3">
-        <v>8.5951849556200003E-3</v>
+        <v>1.8199817340999999E-2</v>
       </c>
       <c r="J3">
-        <v>3.9419416719100001E-2</v>
+        <v>8.4808133087200005E-2</v>
       </c>
       <c r="K3">
-        <v>1.8454770445799999</v>
+        <v>7.0651982380799998</v>
       </c>
       <c r="L3">
-        <v>12</v>
+        <v>43.4782608696</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1385,37 +1101,37 @@
         <v>20</v>
       </c>
       <c r="B4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4">
-        <v>0.66116810854800001</v>
+        <v>0.76653121893300002</v>
       </c>
       <c r="D4">
-        <v>6.6192509572199996E-3</v>
+        <v>1.1713099858E-2</v>
       </c>
       <c r="E4">
-        <v>5.6526102621299999E-2</v>
+        <v>0.121806650574</v>
       </c>
       <c r="F4">
-        <v>4.7828625165499998</v>
+        <v>5.0140741070099999</v>
       </c>
       <c r="G4">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H4">
-        <v>0.50067012711799996</v>
+        <v>0.60103457980300001</v>
       </c>
       <c r="I4">
-        <v>2.0322597248999999E-2</v>
+        <v>2.40321830917E-2</v>
       </c>
       <c r="J4">
-        <v>6.4801797923800003E-2</v>
+        <v>8.0288942447499997E-2</v>
       </c>
       <c r="K4">
-        <v>5.5519357277800001</v>
+        <v>4.8838954369199996</v>
       </c>
       <c r="L4">
-        <v>33.333333333299997</v>
+        <v>26.923076923099998</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1423,37 +1139,37 @@
         <v>20</v>
       </c>
       <c r="B5">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C5">
-        <v>0.70718981657299995</v>
+        <v>0.91305244032300004</v>
       </c>
       <c r="D5">
-        <v>4.4157312563399996E-3</v>
+        <v>8.3438311067200004E-3</v>
       </c>
       <c r="E5">
-        <v>4.8798723183700002E-2</v>
+        <v>7.1740721994100004E-2</v>
       </c>
       <c r="F5">
-        <v>4.2403462727900001</v>
+        <v>3.2474265098599999</v>
       </c>
       <c r="G5">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H5">
-        <v>0.54406367813800005</v>
+        <v>0.74373499092899997</v>
       </c>
       <c r="I5">
-        <v>2.2080718875099999E-2</v>
+        <v>2.1462555802600002E-2</v>
       </c>
       <c r="J5">
-        <v>6.6000801613600002E-2</v>
+        <v>7.5932188199799994E-2</v>
       </c>
       <c r="K5">
-        <v>4.9530275265399997</v>
+        <v>3.9515025854100001</v>
       </c>
       <c r="L5">
-        <v>30.434782608700001</v>
+        <v>22.222222222199999</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1461,37 +1177,37 @@
         <v>20</v>
       </c>
       <c r="B6">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C6">
-        <v>0.849193576678</v>
+        <v>0.76825046896399996</v>
       </c>
       <c r="D6">
-        <v>4.1205882234899996E-3</v>
+        <v>1.19113824813E-2</v>
       </c>
       <c r="E6">
-        <v>2.45778959266E-2</v>
+        <v>0.109555854767</v>
       </c>
       <c r="F6">
-        <v>1.3118741035499999</v>
+        <v>4.8841176033</v>
       </c>
       <c r="G6">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H6">
-        <v>0.68206839715500001</v>
+        <v>0.59893171850600002</v>
       </c>
       <c r="I6">
-        <v>1.45066951716E-2</v>
+        <v>2.4232155747300001E-2</v>
       </c>
       <c r="J6">
-        <v>5.3378125968300001E-2</v>
+        <v>8.5605406799900002E-2</v>
       </c>
       <c r="K6">
-        <v>3.60416736603</v>
+        <v>4.9080296953499998</v>
       </c>
       <c r="L6">
-        <v>29.166666666699999</v>
+        <v>26.923076923099998</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1499,51 +1215,360 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7">
-        <v>0.72252624185100001</v>
+        <v>1.07141887562</v>
       </c>
       <c r="D7">
-        <v>5.0795821555699996E-3</v>
+        <v>5.4874145083499996E-3</v>
       </c>
       <c r="E7">
-        <v>5.8203812775800001E-2</v>
+        <v>2.22521667742E-2</v>
       </c>
       <c r="F7">
-        <v>3.8229811191600001</v>
+        <v>1.2636479437399999</v>
       </c>
       <c r="G7">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H7">
-        <v>0.57134147486099995</v>
+        <v>0.88739298814500001</v>
       </c>
       <c r="I7">
-        <v>2.0224110269799998E-2</v>
+        <v>1.2447388242900001E-2</v>
       </c>
       <c r="J7">
-        <v>6.2203104926000001E-2</v>
+        <v>6.3276118854199995E-2</v>
       </c>
       <c r="K7">
-        <v>4.6641445756</v>
+        <v>2.7461859583899999</v>
       </c>
       <c r="L7">
-        <v>29.166666666699999</v>
+        <v>22.222222222199999</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B8">
         <f>SUM(B2:B7)</f>
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="G8">
         <f>SUM(G2:G7)</f>
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="L8">
         <f>(B8-G8)*100/G8</f>
-        <v>26.388888888888889</v>
+        <v>26.923076923076923</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E90B3B-2217-FD45-B0F5-2A1EC51CEB8D}">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>0.87278514012399999</v>
+      </c>
+      <c r="D2">
+        <v>3.9833604730000003E-3</v>
+      </c>
+      <c r="E2">
+        <v>2.03337562695E-2</v>
+      </c>
+      <c r="F2">
+        <v>1.0280805428799999</v>
+      </c>
+      <c r="G2">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>0.74454854201599996</v>
+      </c>
+      <c r="I2">
+        <v>9.9034918773599993E-3</v>
+      </c>
+      <c r="J2">
+        <v>4.5472811959100003E-2</v>
+      </c>
+      <c r="K2">
+        <v>2.5718787776099998</v>
+      </c>
+      <c r="L2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>32</v>
+      </c>
+      <c r="C3">
+        <v>0.66285055318499997</v>
+      </c>
+      <c r="D3">
+        <v>5.2442033557300004E-3</v>
+      </c>
+      <c r="E3">
+        <v>0.10761772407</v>
+      </c>
+      <c r="F3">
+        <v>4.76998927043</v>
+      </c>
+      <c r="G3">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>0.52964007750099995</v>
+      </c>
+      <c r="I3">
+        <v>1.57053862615E-2</v>
+      </c>
+      <c r="J3">
+        <v>5.7751322660300003E-2</v>
+      </c>
+      <c r="K3">
+        <v>4.8902634657300004</v>
+      </c>
+      <c r="L3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>0.707092986659</v>
+      </c>
+      <c r="D4">
+        <v>3.6918302179699998E-3</v>
+      </c>
+      <c r="E4">
+        <v>9.8789128591800002E-2</v>
+      </c>
+      <c r="F4">
+        <v>4.3708821336400003</v>
+      </c>
+      <c r="G4">
+        <v>24</v>
+      </c>
+      <c r="H4">
+        <v>0.57285710380199995</v>
+      </c>
+      <c r="I4">
+        <v>1.5081766419299999E-2</v>
+      </c>
+      <c r="J4">
+        <v>5.6175789346800002E-2</v>
+      </c>
+      <c r="K4">
+        <v>4.3671628634099999</v>
+      </c>
+      <c r="L4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>0.847756162328</v>
+      </c>
+      <c r="D5">
+        <v>3.5397115085400001E-3</v>
+      </c>
+      <c r="E5">
+        <v>3.9643167790499999E-2</v>
+      </c>
+      <c r="F5">
+        <v>1.360907197</v>
+      </c>
+      <c r="G5">
+        <v>25</v>
+      </c>
+      <c r="H5">
+        <v>0.70579460713499997</v>
+      </c>
+      <c r="I5">
+        <v>1.2127709307899999E-2</v>
+      </c>
+      <c r="J5">
+        <v>4.82150648333E-2</v>
+      </c>
+      <c r="K5">
+        <v>2.9511816024800002</v>
+      </c>
+      <c r="L5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>0.71387954203000004</v>
+      </c>
+      <c r="D6">
+        <v>5.6854001037199998E-3</v>
+      </c>
+      <c r="E6">
+        <v>0.11037950447100001</v>
+      </c>
+      <c r="F6">
+        <v>3.83906775713</v>
+      </c>
+      <c r="G6">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>0.59434208877299999</v>
+      </c>
+      <c r="I6">
+        <v>1.4782525768E-2</v>
+      </c>
+      <c r="J6">
+        <v>5.7164755755300001E-2</v>
+      </c>
+      <c r="K6">
+        <v>4.0905579328500004</v>
+      </c>
+      <c r="L6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>28</v>
+      </c>
+      <c r="C7">
+        <v>0.90750086094399995</v>
+      </c>
+      <c r="D7">
+        <v>2.3249806869499999E-3</v>
+      </c>
+      <c r="E7">
+        <v>1.8440701150199999E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.73760181665400004</v>
+      </c>
+      <c r="G7">
+        <v>26</v>
+      </c>
+      <c r="H7">
+        <v>0.82231857344500003</v>
+      </c>
+      <c r="I7">
+        <v>7.9303806490599992E-3</v>
+      </c>
+      <c r="J7">
+        <v>2.80058384429E-2</v>
+      </c>
+      <c r="K7">
+        <v>1.43126645684</v>
+      </c>
+      <c r="L7">
+        <v>7.69230769231</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <f>SUM(B2:B7)</f>
+        <v>181</v>
+      </c>
+      <c r="G8">
+        <f>SUM(G2:G7)</f>
+        <v>150</v>
+      </c>
+      <c r="L8">
+        <f>(B8-G8)*100/G8</f>
+        <v>20.666666666666668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
graphicsSim doesn't use system time, added results to 25.1, 20.1
</commit_message>
<xml_diff>
--- a/demo_results.xlsx
+++ b/demo_results.xlsx
@@ -8,17 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/serrislew/Desktop/CMU/18-500 Capstone/AutonomousDrivingModels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECE3973-FF07-4E42-BBFE-846C8C88DAB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5283002C-47DE-D540-829B-D1FDBA8D3863}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27880" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="25" sheetId="5" r:id="rId1"/>
-    <sheet name="20" sheetId="6" r:id="rId2"/>
+    <sheet name="25.1" sheetId="7" r:id="rId2"/>
+    <sheet name="20.1" sheetId="8" r:id="rId3"/>
+    <sheet name="20" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="results" localSheetId="1">'20'!$A$1:$L$7</definedName>
+    <definedName name="results" localSheetId="3">'20'!$A$1:$L$7</definedName>
+    <definedName name="results" localSheetId="2">'20.1'!$A$1:$L$7</definedName>
     <definedName name="results" localSheetId="0">'25'!$A$1:$L$7</definedName>
+    <definedName name="results" localSheetId="1">'25.1'!$A$1:$L$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +40,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{4C0F06DF-E766-9A4C-9845-1D2A7DCA8CE9}" name="results1" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{4973B03F-61CA-2340-994B-FC57EC5342AB}" name="results" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="10000" sourceFile="/Users/serrislew/Desktop/CMU/18-500 Capstone/AutonomousDrivingModels/results.csv" comma="1">
       <textFields count="12">
         <textField/>
@@ -54,7 +58,43 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{244D4666-79CD-4D46-B62F-C8FAEBFD2305}" name="results2" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" xr16:uid="{4C0F06DF-E766-9A4C-9845-1D2A7DCA8CE9}" name="results1" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr sourceFile="/Users/serrislew/Desktop/CMU/18-500 Capstone/AutonomousDrivingModels/results.csv" comma="1">
+      <textFields count="12">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" xr16:uid="{244D4666-79CD-4D46-B62F-C8FAEBFD2305}" name="results2" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr sourceFile="/Users/serrislew/Desktop/CMU/18-500 Capstone/AutonomousDrivingModels/results.csv" comma="1">
+      <textFields count="12">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" xr16:uid="{AC7F2A11-ACDE-B541-BB1F-F338ACCD187C}" name="results3" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="10000" sourceFile="/Users/serrislew/Desktop/CMU/18-500 Capstone/AutonomousDrivingModels/results.csv" comma="1">
       <textFields count="12">
         <textField/>
@@ -76,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="20">
   <si>
     <t>Time</t>
   </si>
@@ -113,12 +153,36 @@
   <si>
     <t>Throughput Increase %</t>
   </si>
+  <si>
+    <t>Cooperative</t>
+  </si>
+  <si>
+    <t>Non-cooperative</t>
+  </si>
+  <si>
+    <t>Total Loops</t>
+  </si>
+  <si>
+    <t>Avg Velocity</t>
+  </si>
+  <si>
+    <t>Avg Acceleration</t>
+  </si>
+  <si>
+    <t>Avg Deceleration</t>
+  </si>
+  <si>
+    <t>Avg Waiting Time</t>
+  </si>
+  <si>
+    <t>Percent Increase</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -249,6 +313,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -595,8 +666,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -656,11 +731,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results" connectionId="1" xr16:uid="{1BE21446-64E6-4547-BEA8-04CC74B54DD9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results" connectionId="2" xr16:uid="{1BE21446-64E6-4547-BEA8-04CC74B54DD9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results" connectionId="2" xr16:uid="{EB18F3DE-7027-0F4E-B08C-0E21543D17EE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results" connectionId="1" xr16:uid="{626DEC3E-BCF2-C746-B02C-74899DC1FE0D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results" connectionId="4" xr16:uid="{53FA9663-477F-3349-9461-C799FB344442}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results" connectionId="3" xr16:uid="{EB18F3DE-7027-0F4E-B08C-0E21543D17EE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -960,10 +1043,446 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30DB464B-5D17-F342-B5A9-DB655657D429}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>0.983637105186</v>
+      </c>
+      <c r="D2">
+        <v>6.3752976485100003E-3</v>
+      </c>
+      <c r="E2">
+        <v>6.18717058257E-2</v>
+      </c>
+      <c r="F2">
+        <v>2.4790107939000001</v>
+      </c>
+      <c r="G2">
+        <v>27</v>
+      </c>
+      <c r="H2">
+        <v>0.79590500144499998</v>
+      </c>
+      <c r="I2">
+        <v>1.7345520589300001E-2</v>
+      </c>
+      <c r="J2">
+        <v>7.2813992217499998E-2</v>
+      </c>
+      <c r="K2">
+        <v>3.5153008302100002</v>
+      </c>
+      <c r="L2">
+        <v>22.222222222199999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>0.69806578918899997</v>
+      </c>
+      <c r="D3">
+        <v>1.25092295428E-2</v>
+      </c>
+      <c r="E3">
+        <v>0.125113840591</v>
+      </c>
+      <c r="F3">
+        <v>5.9225344841299998</v>
+      </c>
+      <c r="G3">
+        <v>23</v>
+      </c>
+      <c r="H3">
+        <v>0.45899929867</v>
+      </c>
+      <c r="I3">
+        <v>1.8199817340999999E-2</v>
+      </c>
+      <c r="J3">
+        <v>8.4808133087200005E-2</v>
+      </c>
+      <c r="K3">
+        <v>7.0651982380799998</v>
+      </c>
+      <c r="L3">
+        <v>43.4782608696</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>0.76653121893300002</v>
+      </c>
+      <c r="D4">
+        <v>1.1713099858E-2</v>
+      </c>
+      <c r="E4">
+        <v>0.121806650574</v>
+      </c>
+      <c r="F4">
+        <v>5.0140741070099999</v>
+      </c>
+      <c r="G4">
+        <v>26</v>
+      </c>
+      <c r="H4">
+        <v>0.60103457980300001</v>
+      </c>
+      <c r="I4">
+        <v>2.40321830917E-2</v>
+      </c>
+      <c r="J4">
+        <v>8.0288942447499997E-2</v>
+      </c>
+      <c r="K4">
+        <v>4.8838954369199996</v>
+      </c>
+      <c r="L4">
+        <v>26.923076923099998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>0.91305244032300004</v>
+      </c>
+      <c r="D5">
+        <v>8.3438311067200004E-3</v>
+      </c>
+      <c r="E5">
+        <v>7.1740721994100004E-2</v>
+      </c>
+      <c r="F5">
+        <v>3.2474265098599999</v>
+      </c>
+      <c r="G5">
+        <v>27</v>
+      </c>
+      <c r="H5">
+        <v>0.74373499092899997</v>
+      </c>
+      <c r="I5">
+        <v>2.1462555802600002E-2</v>
+      </c>
+      <c r="J5">
+        <v>7.5932188199799994E-2</v>
+      </c>
+      <c r="K5">
+        <v>3.9515025854100001</v>
+      </c>
+      <c r="L5">
+        <v>22.222222222199999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <v>0.76825046896399996</v>
+      </c>
+      <c r="D6">
+        <v>1.19113824813E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.109555854767</v>
+      </c>
+      <c r="F6">
+        <v>4.8841176033</v>
+      </c>
+      <c r="G6">
+        <v>26</v>
+      </c>
+      <c r="H6">
+        <v>0.59893171850600002</v>
+      </c>
+      <c r="I6">
+        <v>2.4232155747300001E-2</v>
+      </c>
+      <c r="J6">
+        <v>8.5605406799900002E-2</v>
+      </c>
+      <c r="K6">
+        <v>4.9080296953499998</v>
+      </c>
+      <c r="L6">
+        <v>26.923076923099998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <v>1.07141887562</v>
+      </c>
+      <c r="D7">
+        <v>5.4874145083499996E-3</v>
+      </c>
+      <c r="E7">
+        <v>2.22521667742E-2</v>
+      </c>
+      <c r="F7">
+        <v>1.2636479437399999</v>
+      </c>
+      <c r="G7">
+        <v>27</v>
+      </c>
+      <c r="H7">
+        <v>0.88739298814500001</v>
+      </c>
+      <c r="I7">
+        <v>1.2447388242900001E-2</v>
+      </c>
+      <c r="J7">
+        <v>6.3276118854199995E-2</v>
+      </c>
+      <c r="K7">
+        <v>2.7461859583899999</v>
+      </c>
+      <c r="L7">
+        <v>22.222222222199999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <f>SUM(B2:B7)</f>
+        <v>198</v>
+      </c>
+      <c r="C8" s="1">
+        <f>AVERAGE(C2:C7)</f>
+        <v>0.86682598303583325</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" ref="D8:F8" si="0">AVERAGE(D2:D7)</f>
+        <v>9.3900425242800008E-3</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>8.5390156754333327E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>3.8018019069900002</v>
+      </c>
+      <c r="G8" s="1">
+        <f>SUM(G2:G7)</f>
+        <v>156</v>
+      </c>
+      <c r="H8" s="1">
+        <f>AVERAGE(H2:H7)</f>
+        <v>0.68099976291633324</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" ref="I8:K8" si="1">AVERAGE(I2:I7)</f>
+        <v>1.9619936802466667E-2</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="1"/>
+        <v>7.7120796934350005E-2</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5116854573933329</v>
+      </c>
+      <c r="L8" s="1">
+        <f>(B8-G8)*100/G8</f>
+        <v>26.923076923076923</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <f>C8</f>
+        <v>0.86682598303583325</v>
+      </c>
+      <c r="D11">
+        <f>H8</f>
+        <v>0.68099976291633324</v>
+      </c>
+      <c r="E11" s="4">
+        <f>(C11-D11)/D11</f>
+        <v>0.27287266492386486</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <f>D8</f>
+        <v>9.3900425242800008E-3</v>
+      </c>
+      <c r="D12">
+        <f>I8</f>
+        <v>1.9619936802466667E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" ref="E12:E15" si="2">(C12-D12)/D12</f>
+        <v>-0.52140301883645912</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <f>E8</f>
+        <v>8.5390156754333327E-2</v>
+      </c>
+      <c r="D13">
+        <f>J8</f>
+        <v>7.7120796934350005E-2</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.10722606804780184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <f>F8</f>
+        <v>3.8018019069900002</v>
+      </c>
+      <c r="D14">
+        <f>K8</f>
+        <v>4.5116854573933329</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.15734331595303064</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2">
+        <f>B8</f>
+        <v>198</v>
+      </c>
+      <c r="D15" s="2">
+        <v>156</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="2"/>
+        <v>0.26923076923076922</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FACCAB41-7A32-0445-B52F-BBB820D2DC44}">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1025,37 +1544,37 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2">
-        <v>0.983637105186</v>
+        <v>0.99177568466499999</v>
       </c>
       <c r="D2">
-        <v>6.3752976485100003E-3</v>
+        <v>5.1782942421499997E-3</v>
       </c>
       <c r="E2">
-        <v>6.18717058257E-2</v>
+        <v>4.5150299600700002E-2</v>
       </c>
       <c r="F2">
-        <v>2.4790107939000001</v>
+        <v>2.395</v>
       </c>
       <c r="G2">
         <v>27</v>
       </c>
       <c r="H2">
-        <v>0.79590500144499998</v>
+        <v>0.80821873383599996</v>
       </c>
       <c r="I2">
-        <v>1.7345520589300001E-2</v>
+        <v>8.6656385373400004E-3</v>
       </c>
       <c r="J2">
-        <v>7.2813992217499998E-2</v>
+        <v>5.7477820549600003E-2</v>
       </c>
       <c r="K2">
-        <v>3.5153008302100002</v>
+        <v>3.35</v>
       </c>
       <c r="L2">
-        <v>22.222222222199999</v>
+        <v>25.9259259259</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1066,34 +1585,34 @@
         <v>33</v>
       </c>
       <c r="C3">
-        <v>0.69806578918899997</v>
+        <v>0.68774509999800004</v>
       </c>
       <c r="D3">
-        <v>1.25092295428E-2</v>
+        <v>7.9227183176800008E-3</v>
       </c>
       <c r="E3">
-        <v>0.125113840591</v>
+        <v>7.6533715396100002E-2</v>
       </c>
       <c r="F3">
-        <v>5.9225344841299998</v>
+        <v>6.1984615384600001</v>
       </c>
       <c r="G3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H3">
-        <v>0.45899929867</v>
+        <v>0.49475323425399997</v>
       </c>
       <c r="I3">
-        <v>1.8199817340999999E-2</v>
+        <v>8.6434958132499996E-3</v>
       </c>
       <c r="J3">
-        <v>8.4808133087200005E-2</v>
+        <v>5.80429115978E-2</v>
       </c>
       <c r="K3">
-        <v>7.0651982380799998</v>
+        <v>6.1926923076899998</v>
       </c>
       <c r="L3">
-        <v>43.4782608696</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1104,31 +1623,31 @@
         <v>33</v>
       </c>
       <c r="C4">
-        <v>0.76653121893300002</v>
+        <v>0.76789151492499996</v>
       </c>
       <c r="D4">
-        <v>1.1713099858E-2</v>
+        <v>7.3871437340599999E-3</v>
       </c>
       <c r="E4">
-        <v>0.121806650574</v>
+        <v>7.8251613994700001E-2</v>
       </c>
       <c r="F4">
-        <v>5.0140741070099999</v>
+        <v>5.1025</v>
       </c>
       <c r="G4">
         <v>26</v>
       </c>
       <c r="H4">
-        <v>0.60103457980300001</v>
+        <v>0.60804430001800003</v>
       </c>
       <c r="I4">
-        <v>2.40321830917E-2</v>
+        <v>1.0883048921500001E-2</v>
       </c>
       <c r="J4">
-        <v>8.0288942447499997E-2</v>
+        <v>5.5461490303699998E-2</v>
       </c>
       <c r="K4">
-        <v>4.8838954369199996</v>
+        <v>4.4437499999999996</v>
       </c>
       <c r="L4">
         <v>26.923076923099998</v>
@@ -1139,37 +1658,37 @@
         <v>20</v>
       </c>
       <c r="B5">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5">
-        <v>0.91305244032300004</v>
+        <v>0.919835948086</v>
       </c>
       <c r="D5">
-        <v>8.3438311067200004E-3</v>
+        <v>6.2775177858899996E-3</v>
       </c>
       <c r="E5">
-        <v>7.1740721994100004E-2</v>
+        <v>8.2909713526599996E-2</v>
       </c>
       <c r="F5">
-        <v>3.2474265098599999</v>
+        <v>3.2955000000000001</v>
       </c>
       <c r="G5">
         <v>27</v>
       </c>
       <c r="H5">
-        <v>0.74373499092899997</v>
+        <v>0.75151249244100005</v>
       </c>
       <c r="I5">
-        <v>2.1462555802600002E-2</v>
+        <v>9.6458774332000008E-3</v>
       </c>
       <c r="J5">
-        <v>7.5932188199799994E-2</v>
+        <v>5.6051589994199999E-2</v>
       </c>
       <c r="K5">
-        <v>3.9515025854100001</v>
+        <v>3.6735000000000002</v>
       </c>
       <c r="L5">
-        <v>22.222222222199999</v>
+        <v>25.9259259259</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1180,31 +1699,31 @@
         <v>33</v>
       </c>
       <c r="C6">
-        <v>0.76825046896399996</v>
+        <v>0.76894194892699996</v>
       </c>
       <c r="D6">
-        <v>1.19113824813E-2</v>
+        <v>7.6032387720899996E-3</v>
       </c>
       <c r="E6">
-        <v>0.109555854767</v>
+        <v>7.6276907468499994E-2</v>
       </c>
       <c r="F6">
-        <v>4.8841176033</v>
+        <v>4.92875</v>
       </c>
       <c r="G6">
         <v>26</v>
       </c>
       <c r="H6">
-        <v>0.59893171850600002</v>
+        <v>0.61103586777800001</v>
       </c>
       <c r="I6">
-        <v>2.4232155747300001E-2</v>
+        <v>1.03657062532E-2</v>
       </c>
       <c r="J6">
-        <v>8.5605406799900002E-2</v>
+        <v>5.70221275574E-2</v>
       </c>
       <c r="K6">
-        <v>4.9080296953499998</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="L6">
         <v>26.923076923099998</v>
@@ -1215,51 +1734,178 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7">
-        <v>1.07141887562</v>
+        <v>1.09552843897</v>
       </c>
       <c r="D7">
-        <v>5.4874145083499996E-3</v>
+        <v>4.2221665226900001E-3</v>
       </c>
       <c r="E7">
-        <v>2.22521667742E-2</v>
+        <v>1.84805172914E-2</v>
       </c>
       <c r="F7">
-        <v>1.2636479437399999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="G7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H7">
-        <v>0.88739298814500001</v>
+        <v>0.89928702479300004</v>
       </c>
       <c r="I7">
-        <v>1.2447388242900001E-2</v>
+        <v>8.5560144883600007E-3</v>
       </c>
       <c r="J7">
-        <v>6.3276118854199995E-2</v>
+        <v>5.4268538694400001E-2</v>
       </c>
       <c r="K7">
-        <v>2.7461859583899999</v>
+        <v>2.6418750000000002</v>
       </c>
       <c r="L7">
-        <v>22.222222222199999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B8">
+        <v>21.428571428600002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
         <f>SUM(B2:B7)</f>
-        <v>198</v>
-      </c>
-      <c r="G8">
+        <v>201</v>
+      </c>
+      <c r="C8" s="1">
+        <f>AVERAGE(C2:C7)</f>
+        <v>0.87195310592849984</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" ref="D8:F8" si="0">AVERAGE(D2:D7)</f>
+        <v>6.4318465624266666E-3</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>6.2933794546333341E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>3.8433685897433336</v>
+      </c>
+      <c r="G8" s="1">
         <f>SUM(G2:G7)</f>
+        <v>158</v>
+      </c>
+      <c r="H8" s="1">
+        <f>AVERAGE(H2:H7)</f>
+        <v>0.6954752755200001</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" ref="I8:K8" si="1">AVERAGE(I2:I7)</f>
+        <v>9.4599635744749989E-3</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="1"/>
+        <v>5.6387413116183338E-2</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="1"/>
+        <v>4.1211362179483331</v>
+      </c>
+      <c r="L8" s="1">
+        <f>(B8-G8)*100/G8</f>
+        <v>27.215189873417721</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <f>C8</f>
+        <v>0.87195310592849984</v>
+      </c>
+      <c r="D11">
+        <f>H8</f>
+        <v>0.6954752755200001</v>
+      </c>
+      <c r="E11" s="4">
+        <f>(C11-D11)/D11</f>
+        <v>0.25375140802316659</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <f>D8</f>
+        <v>6.4318465624266666E-3</v>
+      </c>
+      <c r="D12">
+        <f>I8</f>
+        <v>9.4599635744749989E-3</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" ref="E12:E15" si="2">(C12-D12)/D12</f>
+        <v>-0.32009816826555637</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <f>E8</f>
+        <v>6.2933794546333341E-2</v>
+      </c>
+      <c r="D13">
+        <f>J8</f>
+        <v>5.6387413116183338E-2</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.11609650218678277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <f>F8</f>
+        <v>3.8433685897433336</v>
+      </c>
+      <c r="D14">
+        <f>K8</f>
+        <v>4.1211362179483331</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="2"/>
+        <v>-6.7400739387178846E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2">
+        <f>B8</f>
+        <v>201</v>
+      </c>
+      <c r="D15" s="2">
         <v>156</v>
       </c>
-      <c r="L8">
-        <f>(B8-G8)*100/G8</f>
-        <v>26.923076923076923</v>
+      <c r="E15" s="4">
+        <f t="shared" si="2"/>
+        <v>0.28846153846153844</v>
       </c>
     </row>
   </sheetData>
@@ -1267,12 +1913,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E90B3B-2217-FD45-B0F5-2A1EC51CEB8D}">
-  <dimension ref="A1:L8"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A299A9B-7E4E-B545-BC2D-A844B1BB626D}">
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1334,37 +1980,37 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2">
-        <v>0.87278514012399999</v>
+        <v>0.88402004599600004</v>
       </c>
       <c r="D2">
-        <v>3.9833604730000003E-3</v>
+        <v>2.5216233674499999E-3</v>
       </c>
       <c r="E2">
-        <v>2.03337562695E-2</v>
+        <v>1.54303167627E-2</v>
       </c>
       <c r="F2">
-        <v>1.0280805428799999</v>
+        <v>0.72166666666699997</v>
       </c>
       <c r="G2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2">
-        <v>0.74454854201599996</v>
+        <v>0.74737291509600001</v>
       </c>
       <c r="I2">
-        <v>9.9034918773599993E-3</v>
+        <v>7.5681151005999999E-3</v>
       </c>
       <c r="J2">
-        <v>4.5472811959100003E-2</v>
+        <v>4.0273186119300003E-2</v>
       </c>
       <c r="K2">
-        <v>2.5718787776099998</v>
+        <v>2.5249999999999999</v>
       </c>
       <c r="L2">
-        <v>20</v>
+        <v>19.2307692308</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1375,31 +2021,31 @@
         <v>32</v>
       </c>
       <c r="C3">
-        <v>0.66285055318499997</v>
+        <v>0.67160727640200002</v>
       </c>
       <c r="D3">
-        <v>5.2442033557300004E-3</v>
+        <v>3.64476300319E-3</v>
       </c>
       <c r="E3">
-        <v>0.10761772407</v>
+        <v>9.1601991862700002E-2</v>
       </c>
       <c r="F3">
-        <v>4.76998927043</v>
+        <v>4.7273076923100001</v>
       </c>
       <c r="G3">
         <v>25</v>
       </c>
       <c r="H3">
-        <v>0.52964007750099995</v>
+        <v>0.53415234567299996</v>
       </c>
       <c r="I3">
-        <v>1.57053862615E-2</v>
+        <v>9.8929012444599999E-3</v>
       </c>
       <c r="J3">
-        <v>5.7751322660300003E-2</v>
+        <v>4.3842334464000002E-2</v>
       </c>
       <c r="K3">
-        <v>4.8902634657300004</v>
+        <v>4.7757692307699999</v>
       </c>
       <c r="L3">
         <v>28</v>
@@ -1410,37 +2056,37 @@
         <v>20</v>
       </c>
       <c r="B4">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4">
-        <v>0.707092986659</v>
+        <v>0.71768834285200001</v>
       </c>
       <c r="D4">
-        <v>3.6918302179699998E-3</v>
+        <v>2.7049495274600001E-3</v>
       </c>
       <c r="E4">
-        <v>9.8789128591800002E-2</v>
+        <v>8.2369549194300007E-2</v>
       </c>
       <c r="F4">
-        <v>4.3708821336400003</v>
+        <v>4.22</v>
       </c>
       <c r="G4">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>0.57756272030900002</v>
+      </c>
+      <c r="I4">
+        <v>1.04498208812E-2</v>
+      </c>
+      <c r="J4">
+        <v>4.5301672241199999E-2</v>
+      </c>
+      <c r="K4">
+        <v>4.25</v>
+      </c>
+      <c r="L4">
         <v>24</v>
-      </c>
-      <c r="H4">
-        <v>0.57285710380199995</v>
-      </c>
-      <c r="I4">
-        <v>1.5081766419299999E-2</v>
-      </c>
-      <c r="J4">
-        <v>5.6175789346800002E-2</v>
-      </c>
-      <c r="K4">
-        <v>4.3671628634099999</v>
-      </c>
-      <c r="L4">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1451,34 +2097,34 @@
         <v>31</v>
       </c>
       <c r="C5">
-        <v>0.847756162328</v>
+        <v>0.85223290071199997</v>
       </c>
       <c r="D5">
-        <v>3.5397115085400001E-3</v>
+        <v>2.8293495775000002E-3</v>
       </c>
       <c r="E5">
-        <v>3.9643167790499999E-2</v>
+        <v>3.4598915671599999E-2</v>
       </c>
       <c r="F5">
-        <v>1.360907197</v>
+        <v>1.2765</v>
       </c>
       <c r="G5">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H5">
-        <v>0.70579460713499997</v>
+        <v>0.70998758893500002</v>
       </c>
       <c r="I5">
-        <v>1.2127709307899999E-2</v>
+        <v>8.7826377746800001E-3</v>
       </c>
       <c r="J5">
-        <v>4.82150648333E-2</v>
+        <v>4.0494611566499999E-2</v>
       </c>
       <c r="K5">
-        <v>2.9511816024800002</v>
+        <v>2.8365</v>
       </c>
       <c r="L5">
-        <v>24</v>
+        <v>19.2307692308</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1486,37 +2132,37 @@
         <v>20</v>
       </c>
       <c r="B6">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C6">
-        <v>0.71387954203000004</v>
+        <v>0.73392184440700003</v>
       </c>
       <c r="D6">
-        <v>5.6854001037199998E-3</v>
+        <v>3.3628767549E-3</v>
       </c>
       <c r="E6">
-        <v>0.11037950447100001</v>
+        <v>7.1193150748400005E-2</v>
       </c>
       <c r="F6">
-        <v>3.83906775713</v>
+        <v>3.6212499999999999</v>
       </c>
       <c r="G6">
         <v>25</v>
       </c>
       <c r="H6">
-        <v>0.59434208877299999</v>
+        <v>0.60393352466500005</v>
       </c>
       <c r="I6">
-        <v>1.4782525768E-2</v>
+        <v>9.9101106871999998E-3</v>
       </c>
       <c r="J6">
-        <v>5.7164755755300001E-2</v>
+        <v>4.36564255038E-2</v>
       </c>
       <c r="K6">
-        <v>4.0905579328500004</v>
+        <v>3.99</v>
       </c>
       <c r="L6">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1527,6 +2173,442 @@
         <v>28</v>
       </c>
       <c r="C7">
+        <v>0.91507543040399997</v>
+      </c>
+      <c r="D7">
+        <v>1.73044674761E-3</v>
+      </c>
+      <c r="E7">
+        <v>1.46742205528E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.72750000000000004</v>
+      </c>
+      <c r="G7">
+        <v>26</v>
+      </c>
+      <c r="H7">
+        <v>0.83802949048599995</v>
+      </c>
+      <c r="I7">
+        <v>5.6922379696199999E-3</v>
+      </c>
+      <c r="J7">
+        <v>1.9632343181599999E-2</v>
+      </c>
+      <c r="K7">
+        <v>1.2524999999999999</v>
+      </c>
+      <c r="L7">
+        <v>7.69230769231</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <f>SUM(B2:B7)</f>
+        <v>185</v>
+      </c>
+      <c r="C8" s="1">
+        <f>AVERAGE(C2:C7)</f>
+        <v>0.79575764012883343</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" ref="D8:F8" si="0">AVERAGE(D2:D7)</f>
+        <v>2.799001496351667E-3</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>5.1644690798750004E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5490373931628336</v>
+      </c>
+      <c r="G8" s="1">
+        <f>SUM(G2:G7)</f>
+        <v>153</v>
+      </c>
+      <c r="H8" s="1">
+        <f>AVERAGE(H2:H7)</f>
+        <v>0.66850643086066663</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" ref="I8:K8" si="1">AVERAGE(I2:I7)</f>
+        <v>8.7159706096266668E-3</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="1"/>
+        <v>3.8866762179400001E-2</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="1"/>
+        <v>3.2716282051283332</v>
+      </c>
+      <c r="L8" s="1">
+        <f>(B8-G8)*100/G8</f>
+        <v>20.915032679738562</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <f>C8</f>
+        <v>0.79575764012883343</v>
+      </c>
+      <c r="D11">
+        <f>H8</f>
+        <v>0.66850643086066663</v>
+      </c>
+      <c r="E11" s="4">
+        <f>(C11-D11)/D11</f>
+        <v>0.19035151106076512</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <f>D8</f>
+        <v>2.799001496351667E-3</v>
+      </c>
+      <c r="D12">
+        <f>I8</f>
+        <v>8.7159706096266668E-3</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" ref="E12:E15" si="2">(C12-D12)/D12</f>
+        <v>-0.67886519795509526</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <f>E8</f>
+        <v>5.1644690798750004E-2</v>
+      </c>
+      <c r="D13">
+        <f>J8</f>
+        <v>3.8866762179400001E-2</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.32876236410869614</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <f>F8</f>
+        <v>2.5490373931628336</v>
+      </c>
+      <c r="D14">
+        <f>K8</f>
+        <v>3.2716282051283332</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.22086580951736084</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2">
+        <f>B8</f>
+        <v>185</v>
+      </c>
+      <c r="D15" s="2">
+        <v>156</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1858974358974359</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E90B3B-2217-FD45-B0F5-2A1EC51CEB8D}">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>0.87278514012399999</v>
+      </c>
+      <c r="D2">
+        <v>3.9833604730000003E-3</v>
+      </c>
+      <c r="E2">
+        <v>2.03337562695E-2</v>
+      </c>
+      <c r="F2">
+        <v>1.0280805428799999</v>
+      </c>
+      <c r="G2">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>0.74454854201599996</v>
+      </c>
+      <c r="I2">
+        <v>9.9034918773599993E-3</v>
+      </c>
+      <c r="J2">
+        <v>4.5472811959100003E-2</v>
+      </c>
+      <c r="K2">
+        <v>2.5718787776099998</v>
+      </c>
+      <c r="L2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>32</v>
+      </c>
+      <c r="C3">
+        <v>0.66285055318499997</v>
+      </c>
+      <c r="D3">
+        <v>5.2442033557300004E-3</v>
+      </c>
+      <c r="E3">
+        <v>0.10761772407</v>
+      </c>
+      <c r="F3">
+        <v>4.76998927043</v>
+      </c>
+      <c r="G3">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>0.52964007750099995</v>
+      </c>
+      <c r="I3">
+        <v>1.57053862615E-2</v>
+      </c>
+      <c r="J3">
+        <v>5.7751322660300003E-2</v>
+      </c>
+      <c r="K3">
+        <v>4.8902634657300004</v>
+      </c>
+      <c r="L3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>0.707092986659</v>
+      </c>
+      <c r="D4">
+        <v>3.6918302179699998E-3</v>
+      </c>
+      <c r="E4">
+        <v>9.8789128591800002E-2</v>
+      </c>
+      <c r="F4">
+        <v>4.3708821336400003</v>
+      </c>
+      <c r="G4">
+        <v>24</v>
+      </c>
+      <c r="H4">
+        <v>0.57285710380199995</v>
+      </c>
+      <c r="I4">
+        <v>1.5081766419299999E-2</v>
+      </c>
+      <c r="J4">
+        <v>5.6175789346800002E-2</v>
+      </c>
+      <c r="K4">
+        <v>4.3671628634099999</v>
+      </c>
+      <c r="L4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>0.847756162328</v>
+      </c>
+      <c r="D5">
+        <v>3.5397115085400001E-3</v>
+      </c>
+      <c r="E5">
+        <v>3.9643167790499999E-2</v>
+      </c>
+      <c r="F5">
+        <v>1.360907197</v>
+      </c>
+      <c r="G5">
+        <v>25</v>
+      </c>
+      <c r="H5">
+        <v>0.70579460713499997</v>
+      </c>
+      <c r="I5">
+        <v>1.2127709307899999E-2</v>
+      </c>
+      <c r="J5">
+        <v>4.82150648333E-2</v>
+      </c>
+      <c r="K5">
+        <v>2.9511816024800002</v>
+      </c>
+      <c r="L5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>0.71387954203000004</v>
+      </c>
+      <c r="D6">
+        <v>5.6854001037199998E-3</v>
+      </c>
+      <c r="E6">
+        <v>0.11037950447100001</v>
+      </c>
+      <c r="F6">
+        <v>3.83906775713</v>
+      </c>
+      <c r="G6">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>0.59434208877299999</v>
+      </c>
+      <c r="I6">
+        <v>1.4782525768E-2</v>
+      </c>
+      <c r="J6">
+        <v>5.7164755755300001E-2</v>
+      </c>
+      <c r="K6">
+        <v>4.0905579328500004</v>
+      </c>
+      <c r="L6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>28</v>
+      </c>
+      <c r="C7">
         <v>0.90750086094399995</v>
       </c>
       <c r="D7">
@@ -1557,18 +2639,145 @@
         <v>7.69230769231</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B8">
+    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
         <f>SUM(B2:B7)</f>
         <v>181</v>
       </c>
-      <c r="G8">
+      <c r="C8" s="1">
+        <f>AVERAGE(C2:C7)</f>
+        <v>0.78531087421166668</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" ref="D8:F8" si="0">AVERAGE(D2:D7)</f>
+        <v>4.0782477243183337E-3</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>6.5867330390500009E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6844214529556663</v>
+      </c>
+      <c r="G8" s="1">
         <f>SUM(G2:G7)</f>
         <v>150</v>
       </c>
-      <c r="L8">
+      <c r="H8" s="1">
+        <f>AVERAGE(H2:H7)</f>
+        <v>0.66158349877866662</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" ref="I8:K8" si="1">AVERAGE(I2:I7)</f>
+        <v>1.258854338052E-2</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="1"/>
+        <v>4.8797597166283339E-2</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="1"/>
+        <v>3.3837185164866668</v>
+      </c>
+      <c r="L8" s="1">
         <f>(B8-G8)*100/G8</f>
         <v>20.666666666666668</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <f>C8</f>
+        <v>0.78531087421166668</v>
+      </c>
+      <c r="D11">
+        <f>H8</f>
+        <v>0.66158349877866662</v>
+      </c>
+      <c r="E11" s="4">
+        <f>(C11-D11)/D11</f>
+        <v>0.18701702152700328</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <f>D8</f>
+        <v>4.0782477243183337E-3</v>
+      </c>
+      <c r="D12">
+        <f>I8</f>
+        <v>1.258854338052E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" ref="E12:E15" si="2">(C12-D12)/D12</f>
+        <v>-0.67603497870697482</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <f>E8</f>
+        <v>6.5867330390500009E-2</v>
+      </c>
+      <c r="D13">
+        <f>J8</f>
+        <v>4.8797597166283339E-2</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.34980683917795419</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <f>F8</f>
+        <v>2.6844214529556663</v>
+      </c>
+      <c r="D14">
+        <f>K8</f>
+        <v>3.3837185164866668</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.20666525898173246</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2">
+        <f>B8</f>
+        <v>181</v>
+      </c>
+      <c r="D15" s="2">
+        <v>156</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="2"/>
+        <v>0.16025641025641027</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update results using new metrics
</commit_message>
<xml_diff>
--- a/demo_results.xlsx
+++ b/demo_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyleesantos/Documents/AutonomousDrivingModels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0F6147-C68E-F74D-89D8-4A949946D74D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAB747F-9EC2-4945-9641-82EF18D98553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,6 @@
   <definedNames>
     <definedName name="results" localSheetId="3">'20'!$A$1:$L$7</definedName>
     <definedName name="results" localSheetId="2">'20.1'!$A$1:$L$7</definedName>
-    <definedName name="results" localSheetId="0">'25'!$A$1:$L$7</definedName>
     <definedName name="results" localSheetId="1">'25.1'!$A$1:$L$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -58,7 +57,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{4C0F06DF-E766-9A4C-9845-1D2A7DCA8CE9}" name="results1" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" xr16:uid="{244D4666-79CD-4D46-B62F-C8FAEBFD2305}" name="results2" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr sourceFile="/Users/serrislew/Desktop/CMU/18-500 Capstone/AutonomousDrivingModels/results.csv" comma="1">
       <textFields count="12">
         <textField/>
@@ -76,25 +75,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{244D4666-79CD-4D46-B62F-C8FAEBFD2305}" name="results2" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr sourceFile="/Users/serrislew/Desktop/CMU/18-500 Capstone/AutonomousDrivingModels/results.csv" comma="1">
-      <textFields count="12">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="4" xr16:uid="{AC7F2A11-ACDE-B541-BB1F-F338ACCD187C}" name="results3" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="3" xr16:uid="{AC7F2A11-ACDE-B541-BB1F-F338ACCD187C}" name="results3" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr sourceFile="/Users/serrislew/Desktop/CMU/18-500 Capstone/AutonomousDrivingModels/results.csv" comma="1">
       <textFields count="12">
         <textField/>
@@ -116,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="29">
   <si>
     <t>Time</t>
   </si>
@@ -176,6 +157,33 @@
   </si>
   <si>
     <t>Percent Increase</t>
+  </si>
+  <si>
+    <t>Coop Net Average Acceleration</t>
+  </si>
+  <si>
+    <t>Coop Total Count Acceleration</t>
+  </si>
+  <si>
+    <t>Coop Total Count Deceleration</t>
+  </si>
+  <si>
+    <t>Non-Coop Net Average Acceleration</t>
+  </si>
+  <si>
+    <t>Non-Coop Total Count Acceleration</t>
+  </si>
+  <si>
+    <t>Non-Coop Total Count Deceleration</t>
+  </si>
+  <si>
+    <t>Avg Net Accel.</t>
+  </si>
+  <si>
+    <t>Avg Accel Counts</t>
+  </si>
+  <si>
+    <t>Avg Decel Counts</t>
   </si>
 </sst>
 </file>
@@ -732,19 +740,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results" connectionId="2" xr16:uid="{1BE21446-64E6-4547-BEA8-04CC74B54DD9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results" connectionId="1" xr16:uid="{626DEC3E-BCF2-C746-B02C-74899DC1FE0D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results" connectionId="1" xr16:uid="{626DEC3E-BCF2-C746-B02C-74899DC1FE0D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results" connectionId="3" xr16:uid="{53FA9663-477F-3349-9461-C799FB344442}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results" connectionId="4" xr16:uid="{53FA9663-477F-3349-9461-C799FB344442}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results" connectionId="3" xr16:uid="{EB18F3DE-7027-0F4E-B08C-0E21543D17EE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results" connectionId="2" xr16:uid="{EB18F3DE-7027-0F4E-B08C-0E21543D17EE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1044,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30DB464B-5D17-F342-B5A9-DB655657D429}">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1064,9 +1068,10 @@
     <col min="10" max="10" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1077,34 +1082,52 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>40</v>
       </c>
@@ -1115,43 +1138,61 @@
         <v>0.841274905251302</v>
       </c>
       <c r="D2">
+        <v>1.3599999999999901</v>
+      </c>
+      <c r="E2">
         <v>1.8210966067681099E-2</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.116789837731996</v>
       </c>
-      <c r="F2">
-        <v>1.3599999999999901</v>
-      </c>
       <c r="G2">
+        <v>-9.8578871664315004E-2</v>
+      </c>
+      <c r="H2">
+        <v>154.888888888888</v>
+      </c>
+      <c r="I2">
+        <v>1350</v>
+      </c>
+      <c r="J2">
         <v>46</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <v>0.68415394914007099</v>
       </c>
-      <c r="I2">
+      <c r="L2">
+        <v>6.7449999999999601</v>
+      </c>
+      <c r="M2">
         <v>1.7484960951841801E-2</v>
       </c>
-      <c r="J2">
+      <c r="N2">
         <v>0.15233644845633401</v>
       </c>
-      <c r="K2">
-        <v>6.7449999999999601</v>
-      </c>
-      <c r="L2">
+      <c r="O2">
+        <v>-0.134851487504492</v>
+      </c>
+      <c r="P2">
+        <v>297.666666666666</v>
+      </c>
+      <c r="Q2">
+        <v>1475.3333333333301</v>
+      </c>
+      <c r="R2">
         <v>23.9130434782608</v>
       </c>
-      <c r="O2" t="s">
+      <c r="U2" t="s">
         <v>12</v>
       </c>
-      <c r="P2" t="s">
+      <c r="V2" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="W2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>40</v>
       </c>
@@ -1162,49 +1203,67 @@
         <v>0.64403373856100199</v>
       </c>
       <c r="D3">
+        <v>9.3080769230769</v>
+      </c>
+      <c r="E3">
         <v>2.1616551609404101E-2</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.27724911401984897</v>
       </c>
-      <c r="F3">
-        <v>9.3080769230769</v>
-      </c>
       <c r="G3">
+        <v>-0.25563256241044502</v>
+      </c>
+      <c r="H3">
+        <v>218.15384615384599</v>
+      </c>
+      <c r="I3">
+        <v>1634.76923076923</v>
+      </c>
+      <c r="J3">
         <v>46</v>
       </c>
-      <c r="H3">
+      <c r="K3">
         <v>0.4807867934408</v>
       </c>
-      <c r="I3">
+      <c r="L3">
+        <v>11.1957692307692</v>
+      </c>
+      <c r="M3">
         <v>1.36974504926867E-2</v>
       </c>
-      <c r="J3">
+      <c r="N3">
         <v>0.102965611791248</v>
       </c>
-      <c r="K3">
-        <v>11.1957692307692</v>
-      </c>
-      <c r="L3">
+      <c r="O3">
+        <v>-8.9268161298561202E-2</v>
+      </c>
+      <c r="P3">
+        <v>735.38461538461502</v>
+      </c>
+      <c r="Q3">
+        <v>1530.76923076923</v>
+      </c>
+      <c r="R3">
         <v>34.782608695652101</v>
       </c>
-      <c r="N3" t="s">
+      <c r="T3" t="s">
         <v>15</v>
       </c>
-      <c r="O3">
+      <c r="U3">
         <f>C52</f>
         <v>0.75437994234678896</v>
       </c>
-      <c r="P3">
-        <f>H52</f>
+      <c r="V3">
+        <f>K52</f>
         <v>0.58828403089339754</v>
       </c>
-      <c r="Q3" s="4">
-        <f>(O3-P3)/P3</f>
+      <c r="W3" s="4">
+        <f>(U3-V3)/V3</f>
         <v>0.28233965691903939</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>40</v>
       </c>
@@ -1215,49 +1274,67 @@
         <v>0.69035826711667603</v>
       </c>
       <c r="D4">
+        <v>8.2099999999999493</v>
+      </c>
+      <c r="E4">
         <v>1.98133609246561E-2</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.25802447042058202</v>
       </c>
-      <c r="F4">
-        <v>8.2099999999999493</v>
-      </c>
       <c r="G4">
+        <v>-0.238211109495926</v>
+      </c>
+      <c r="H4">
+        <v>169.75</v>
+      </c>
+      <c r="I4">
+        <v>1595.3333333333301</v>
+      </c>
+      <c r="J4">
         <v>45</v>
       </c>
-      <c r="H4">
+      <c r="K4">
         <v>0.52088820561594895</v>
       </c>
-      <c r="I4">
+      <c r="L4">
+        <v>10.06875</v>
+      </c>
+      <c r="M4">
         <v>1.41548442432145E-2</v>
       </c>
-      <c r="J4">
+      <c r="N4">
         <v>0.110015991529861</v>
       </c>
-      <c r="K4">
-        <v>10.06875</v>
-      </c>
-      <c r="L4">
+      <c r="O4">
+        <v>-9.5861147286647297E-2</v>
+      </c>
+      <c r="P4">
+        <v>685.75</v>
+      </c>
+      <c r="Q4">
+        <v>1511.5833333333301</v>
+      </c>
+      <c r="R4">
         <v>33.3333333333333</v>
       </c>
-      <c r="N4" t="s">
+      <c r="T4" t="s">
         <v>16</v>
       </c>
-      <c r="O4">
-        <f>D52</f>
+      <c r="U4">
+        <f>E52</f>
         <v>1.9663948276889193E-2</v>
       </c>
-      <c r="P4">
-        <f>I52</f>
+      <c r="V4">
+        <f>M52</f>
         <v>1.4981833987919729E-2</v>
       </c>
-      <c r="Q4" s="3">
-        <f t="shared" ref="Q4:Q7" si="0">(O4-P4)/P4</f>
+      <c r="W4" s="4">
+        <f>(U4-V4)/V4</f>
         <v>0.31251943471972682</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>40</v>
       </c>
@@ -1268,49 +1345,67 @@
         <v>0.80959253841119505</v>
       </c>
       <c r="D5">
+        <v>2.5904999999999898</v>
+      </c>
+      <c r="E5">
         <v>1.5555730161051299E-2</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.14790677109640599</v>
       </c>
-      <c r="F5">
-        <v>2.5904999999999898</v>
-      </c>
       <c r="G5">
+        <v>-0.13235104093535399</v>
+      </c>
+      <c r="H5">
+        <v>181.2</v>
+      </c>
+      <c r="I5">
+        <v>1415.4</v>
+      </c>
+      <c r="J5">
         <v>46</v>
       </c>
-      <c r="H5">
+      <c r="K5">
         <v>0.63027958025706998</v>
       </c>
-      <c r="I5">
+      <c r="L5">
+        <v>8.2229999999999297</v>
+      </c>
+      <c r="M5">
         <v>1.49805990755566E-2</v>
       </c>
-      <c r="J5">
+      <c r="N5">
         <v>0.125303247804192</v>
       </c>
-      <c r="K5">
-        <v>8.2229999999999297</v>
-      </c>
-      <c r="L5">
+      <c r="O5">
+        <v>-0.11032264872863599</v>
+      </c>
+      <c r="P5">
+        <v>381.3</v>
+      </c>
+      <c r="Q5">
+        <v>1531.9</v>
+      </c>
+      <c r="R5">
         <v>30.434782608695599</v>
       </c>
-      <c r="N5" t="s">
+      <c r="T5" t="s">
         <v>17</v>
       </c>
-      <c r="O5">
-        <f>E52</f>
+      <c r="U5">
+        <f>F52</f>
         <v>0.26652864826233214</v>
       </c>
-      <c r="P5">
-        <f>J52</f>
+      <c r="V5">
+        <f>N52</f>
         <v>0.15050920535299253</v>
       </c>
-      <c r="Q5" s="4">
-        <f t="shared" si="0"/>
+      <c r="W5" s="4">
+        <f>(U5-V5)/V5</f>
         <v>0.77084615945740109</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>40</v>
       </c>
@@ -1321,49 +1416,67 @@
         <v>0.70034154245700997</v>
       </c>
       <c r="D6">
+        <v>7.6637499999999603</v>
+      </c>
+      <c r="E6">
         <v>1.91046686863999E-2</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0.24690730742153999</v>
       </c>
-      <c r="F6">
-        <v>7.6637499999999603</v>
-      </c>
       <c r="G6">
+        <v>-0.22780263873514001</v>
+      </c>
+      <c r="H6">
+        <v>172.583333333333</v>
+      </c>
+      <c r="I6">
+        <v>1557.1666666666599</v>
+      </c>
+      <c r="J6">
         <v>46</v>
       </c>
-      <c r="H6">
+      <c r="K6">
         <v>0.53438148624475101</v>
       </c>
-      <c r="I6">
+      <c r="L6">
+        <v>9.8049999999999908</v>
+      </c>
+      <c r="M6">
         <v>1.3638996050123E-2</v>
       </c>
-      <c r="J6">
+      <c r="N6">
         <v>0.109678242997178</v>
       </c>
-      <c r="K6">
-        <v>9.8049999999999908</v>
-      </c>
-      <c r="L6">
+      <c r="O6">
+        <v>-9.6039246947055706E-2</v>
+      </c>
+      <c r="P6">
+        <v>665.5</v>
+      </c>
+      <c r="Q6">
+        <v>1498.75</v>
+      </c>
+      <c r="R6">
         <v>32.6086956521739</v>
       </c>
-      <c r="N6" t="s">
-        <v>18</v>
-      </c>
-      <c r="O6">
-        <f>F52</f>
-        <v>4.9310199883449695</v>
-      </c>
-      <c r="P6">
-        <f>K52</f>
-        <v>8.7865401981351745</v>
-      </c>
-      <c r="Q6" s="3">
-        <f t="shared" si="0"/>
-        <v>-0.43879844886027924</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T6" t="s">
+        <v>26</v>
+      </c>
+      <c r="U6">
+        <f>G52</f>
+        <v>-0.24686469998544289</v>
+      </c>
+      <c r="V6">
+        <f>O52</f>
+        <v>-0.1355273713650729</v>
+      </c>
+      <c r="W6" s="3">
+        <f>(U6-V6)/ABS(V6)</f>
+        <v>-0.82151175440758983</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>40</v>
       </c>
@@ -1374,163 +1487,280 @@
         <v>0.87100660826832998</v>
       </c>
       <c r="D7">
+        <v>0.97833333333333194</v>
+      </c>
+      <c r="E7">
         <v>1.52387240726623E-2</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>0.104404268519007</v>
       </c>
-      <c r="F7">
-        <v>0.97833333333333194</v>
-      </c>
       <c r="G7">
+        <v>-8.9165544446345196E-2</v>
+      </c>
+      <c r="H7">
+        <v>120.555555555555</v>
+      </c>
+      <c r="I7">
+        <v>1293.2222222222199</v>
+      </c>
+      <c r="J7">
         <v>46</v>
       </c>
-      <c r="H7">
+      <c r="K7">
         <v>0.67868018457941603</v>
       </c>
-      <c r="I7">
+      <c r="L7">
+        <v>6.8816666666666304</v>
+      </c>
+      <c r="M7">
         <v>1.81758865055788E-2</v>
       </c>
-      <c r="J7">
+      <c r="N7">
         <v>0.149744491407928</v>
       </c>
-      <c r="K7">
-        <v>6.8816666666666304</v>
-      </c>
-      <c r="L7">
+      <c r="O7">
+        <v>-0.13156860490235001</v>
+      </c>
+      <c r="P7">
+        <v>307.666666666666</v>
+      </c>
+      <c r="Q7">
+        <v>1484.2222222222199</v>
+      </c>
+      <c r="R7">
         <v>28.260869565217298</v>
       </c>
-      <c r="N7" t="s">
+      <c r="T7" t="s">
+        <v>27</v>
+      </c>
+      <c r="U7" s="2">
+        <f>H52</f>
+        <v>195.21977544677506</v>
+      </c>
+      <c r="V7" s="2">
+        <f>P52</f>
+        <v>515.77030536130519</v>
+      </c>
+      <c r="W7" s="3">
+        <f>(U7-V7)/V7</f>
+        <v>-0.62149861398084838</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <v>56</v>
+      </c>
+      <c r="C8">
+        <v>0.8570636686309</v>
+      </c>
+      <c r="D8">
+        <v>0.81666666666666599</v>
+      </c>
+      <c r="E8">
+        <v>1.8654835984292201E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.111235990782522</v>
+      </c>
+      <c r="G8">
+        <v>-9.2581154798229898E-2</v>
+      </c>
+      <c r="H8">
+        <v>161.111111111111</v>
+      </c>
+      <c r="I8">
+        <v>1310.3333333333301</v>
+      </c>
+      <c r="J8">
+        <v>47</v>
+      </c>
+      <c r="K8">
+        <v>0.71682698811606405</v>
+      </c>
+      <c r="L8">
+        <v>5.7266666666666302</v>
+      </c>
+      <c r="M8">
+        <v>1.6905765649537399E-2</v>
+      </c>
+      <c r="N8">
+        <v>0.146721213943555</v>
+      </c>
+      <c r="O8">
+        <v>-0.12981544829401701</v>
+      </c>
+      <c r="P8">
+        <v>285.888888888888</v>
+      </c>
+      <c r="Q8">
+        <v>1417.55555555555</v>
+      </c>
+      <c r="R8">
+        <v>19.1489361702127</v>
+      </c>
+      <c r="T8" t="s">
+        <v>28</v>
+      </c>
+      <c r="U8" s="2">
+        <f>I52</f>
+        <v>1463.2749704739663</v>
+      </c>
+      <c r="V8" s="2">
+        <f>Q52</f>
+        <v>1497.5419487179449</v>
+      </c>
+      <c r="W8" s="3">
+        <f>(U8-V8)/V8</f>
+        <v>-2.2882149160038442E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>40</v>
+      </c>
+      <c r="B9">
+        <v>62</v>
+      </c>
+      <c r="C9">
+        <v>0.64935365807126699</v>
+      </c>
+      <c r="D9">
+        <v>9.0126923076922907</v>
+      </c>
+      <c r="E9">
+        <v>2.2951702987491801E-2</v>
+      </c>
+      <c r="F9">
+        <v>0.27339571281278702</v>
+      </c>
+      <c r="G9">
+        <v>-0.25044400982529602</v>
+      </c>
+      <c r="H9">
+        <v>225.461538461538</v>
+      </c>
+      <c r="I9">
+        <v>1626.8461538461499</v>
+      </c>
+      <c r="J9">
+        <v>46</v>
+      </c>
+      <c r="K9">
+        <v>0.490939187787858</v>
+      </c>
+      <c r="L9">
+        <v>11.0088461538461</v>
+      </c>
+      <c r="M9">
+        <v>1.36393634825066E-2</v>
+      </c>
+      <c r="N9">
+        <v>0.106362659287841</v>
+      </c>
+      <c r="O9">
+        <v>-9.2723295805334505E-2</v>
+      </c>
+      <c r="P9">
+        <v>710</v>
+      </c>
+      <c r="Q9">
+        <v>1526.6923076922999</v>
+      </c>
+      <c r="R9">
+        <v>34.782608695652101</v>
+      </c>
+      <c r="T9" t="s">
+        <v>18</v>
+      </c>
+      <c r="U9">
+        <f>D52</f>
+        <v>4.9310199883449695</v>
+      </c>
+      <c r="V9">
+        <f>L52</f>
+        <v>8.7865401981351745</v>
+      </c>
+      <c r="W9" s="3">
+        <f>(U9-V9)/V9</f>
+        <v>-0.43879844886027924</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>40</v>
+      </c>
+      <c r="B10">
+        <v>57</v>
+      </c>
+      <c r="C10">
+        <v>0.85387931357620495</v>
+      </c>
+      <c r="D10">
+        <v>0.87833333333333297</v>
+      </c>
+      <c r="E10">
+        <v>1.7776376963596501E-2</v>
+      </c>
+      <c r="F10">
+        <v>0.105299993084383</v>
+      </c>
+      <c r="G10">
+        <v>-8.7523616120787295E-2</v>
+      </c>
+      <c r="H10">
+        <v>163.111111111111</v>
+      </c>
+      <c r="I10">
+        <v>1326.7777777777701</v>
+      </c>
+      <c r="J10">
+        <v>46</v>
+      </c>
+      <c r="K10">
+        <v>0.70333697461760403</v>
+      </c>
+      <c r="L10">
+        <v>6.2966666666666198</v>
+      </c>
+      <c r="M10">
+        <v>1.8062537438134501E-2</v>
+      </c>
+      <c r="N10">
+        <v>0.14756240127020001</v>
+      </c>
+      <c r="O10">
+        <v>-0.12949986383206599</v>
+      </c>
+      <c r="P10">
+        <v>276.11111111111097</v>
+      </c>
+      <c r="Q10">
+        <v>1461.1111111111099</v>
+      </c>
+      <c r="R10">
+        <v>23.9130434782608</v>
+      </c>
+      <c r="T10" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="2">
+      <c r="U10" s="2">
         <f>B52</f>
         <v>3004</v>
       </c>
-      <c r="P7" s="2">
-        <f>G52</f>
+      <c r="V10" s="2">
+        <f>J52</f>
         <v>2305</v>
       </c>
-      <c r="Q7" s="4">
-        <f t="shared" si="0"/>
+      <c r="W10" s="4">
+        <f>(U10-V10)/V10</f>
         <v>0.30325379609544467</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>40</v>
-      </c>
-      <c r="B8">
-        <v>56</v>
-      </c>
-      <c r="C8">
-        <v>0.8570636686309</v>
-      </c>
-      <c r="D8">
-        <v>1.8654835984292201E-2</v>
-      </c>
-      <c r="E8">
-        <v>0.111235990782522</v>
-      </c>
-      <c r="F8">
-        <v>0.81666666666666599</v>
-      </c>
-      <c r="G8">
-        <v>47</v>
-      </c>
-      <c r="H8">
-        <v>0.71682698811606405</v>
-      </c>
-      <c r="I8">
-        <v>1.6905765649537399E-2</v>
-      </c>
-      <c r="J8">
-        <v>0.146721213943555</v>
-      </c>
-      <c r="K8">
-        <v>5.7266666666666302</v>
-      </c>
-      <c r="L8">
-        <v>19.1489361702127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>40</v>
-      </c>
-      <c r="B9">
-        <v>62</v>
-      </c>
-      <c r="C9">
-        <v>0.64935365807126699</v>
-      </c>
-      <c r="D9">
-        <v>2.2951702987491801E-2</v>
-      </c>
-      <c r="E9">
-        <v>0.27339571281278702</v>
-      </c>
-      <c r="F9">
-        <v>9.0126923076922907</v>
-      </c>
-      <c r="G9">
-        <v>46</v>
-      </c>
-      <c r="H9">
-        <v>0.490939187787858</v>
-      </c>
-      <c r="I9">
-        <v>1.36393634825066E-2</v>
-      </c>
-      <c r="J9">
-        <v>0.106362659287841</v>
-      </c>
-      <c r="K9">
-        <v>11.0088461538461</v>
-      </c>
-      <c r="L9">
-        <v>34.782608695652101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>40</v>
-      </c>
-      <c r="B10">
-        <v>57</v>
-      </c>
-      <c r="C10">
-        <v>0.85387931357620495</v>
-      </c>
-      <c r="D10">
-        <v>1.7776376963596501E-2</v>
-      </c>
-      <c r="E10">
-        <v>0.105299993084383</v>
-      </c>
-      <c r="F10">
-        <v>0.87833333333333297</v>
-      </c>
-      <c r="G10">
-        <v>46</v>
-      </c>
-      <c r="H10">
-        <v>0.70333697461760403</v>
-      </c>
-      <c r="I10">
-        <v>1.8062537438134501E-2</v>
-      </c>
-      <c r="J10">
-        <v>0.14756240127020001</v>
-      </c>
-      <c r="K10">
-        <v>6.2966666666666198</v>
-      </c>
-      <c r="L10">
-        <v>23.9130434782608</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>40</v>
       </c>
@@ -1541,34 +1771,52 @@
         <v>0.853699347849463</v>
       </c>
       <c r="D11">
+        <v>0.96666666666666601</v>
+      </c>
+      <c r="E11">
         <v>1.7506835858390999E-2</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>0.107404816661878</v>
       </c>
-      <c r="F11">
-        <v>0.96666666666666601</v>
-      </c>
       <c r="G11">
+        <v>-8.9897980803487904E-2</v>
+      </c>
+      <c r="H11">
+        <v>158.666666666666</v>
+      </c>
+      <c r="I11">
+        <v>1315.2222222222199</v>
+      </c>
+      <c r="J11">
         <v>46</v>
       </c>
-      <c r="H11">
+      <c r="K11">
         <v>0.69497752422710202</v>
       </c>
-      <c r="I11">
+      <c r="L11">
+        <v>6.4833333333332899</v>
+      </c>
+      <c r="M11">
         <v>1.7527076421699001E-2</v>
       </c>
-      <c r="J11">
+      <c r="N11">
         <v>0.15128215453792301</v>
       </c>
-      <c r="K11">
-        <v>6.4833333333332899</v>
-      </c>
-      <c r="L11">
+      <c r="O11">
+        <v>-0.133755078116224</v>
+      </c>
+      <c r="P11">
+        <v>284.666666666666</v>
+      </c>
+      <c r="Q11">
+        <v>1474.2222222222199</v>
+      </c>
+      <c r="R11">
         <v>23.9130434782608</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>40</v>
       </c>
@@ -1579,34 +1827,52 @@
         <v>0.85879147790884802</v>
       </c>
       <c r="D12">
+        <v>0.70333333333333303</v>
+      </c>
+      <c r="E12">
         <v>1.9577348337661001E-2</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>0.10533281311953301</v>
       </c>
-      <c r="F12">
-        <v>0.70333333333333303</v>
-      </c>
       <c r="G12">
+        <v>-8.5755464781872806E-2</v>
+      </c>
+      <c r="H12">
+        <v>161.444444444444</v>
+      </c>
+      <c r="I12">
+        <v>1323.44444444444</v>
+      </c>
+      <c r="J12">
         <v>46</v>
       </c>
-      <c r="H12">
+      <c r="K12">
         <v>0.71226989623276604</v>
       </c>
-      <c r="I12">
+      <c r="L12">
+        <v>5.9266666666666303</v>
+      </c>
+      <c r="M12">
         <v>1.6808075736650802E-2</v>
       </c>
-      <c r="J12">
+      <c r="N12">
         <v>0.14406894793413999</v>
       </c>
-      <c r="K12">
-        <v>5.9266666666666303</v>
-      </c>
-      <c r="L12">
+      <c r="O12">
+        <v>-0.12726087219748899</v>
+      </c>
+      <c r="P12">
+        <v>279.77777777777698</v>
+      </c>
+      <c r="Q12">
+        <v>1436.44444444444</v>
+      </c>
+      <c r="R12">
         <v>23.9130434782608</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>40</v>
       </c>
@@ -1617,34 +1883,52 @@
         <v>0.85140650169833298</v>
       </c>
       <c r="D13">
+        <v>1.0249999999999899</v>
+      </c>
+      <c r="E13">
         <v>1.75036876890057E-2</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>0.108417602333877</v>
       </c>
-      <c r="F13">
-        <v>1.0249999999999899</v>
-      </c>
       <c r="G13">
+        <v>-9.0913914644871502E-2</v>
+      </c>
+      <c r="H13">
+        <v>160.888888888888</v>
+      </c>
+      <c r="I13">
+        <v>1329.6666666666599</v>
+      </c>
+      <c r="J13">
         <v>46</v>
       </c>
-      <c r="H13">
+      <c r="K13">
         <v>0.70273447465926298</v>
       </c>
-      <c r="I13">
+      <c r="L13">
+        <v>6.2366666666666299</v>
+      </c>
+      <c r="M13">
         <v>1.7440671262609501E-2</v>
       </c>
-      <c r="J13">
+      <c r="N13">
         <v>0.14842933438578301</v>
       </c>
-      <c r="K13">
-        <v>6.2366666666666299</v>
-      </c>
-      <c r="L13">
+      <c r="O13">
+        <v>-0.130988663123173</v>
+      </c>
+      <c r="P13">
+        <v>285</v>
+      </c>
+      <c r="Q13">
+        <v>1455.88888888888</v>
+      </c>
+      <c r="R13">
         <v>23.9130434782608</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>40</v>
       </c>
@@ -1655,34 +1939,52 @@
         <v>0.84313924374152605</v>
       </c>
       <c r="D14">
+        <v>1.04849999999999</v>
+      </c>
+      <c r="E14">
         <v>2.3729164625692901E-2</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>0.111863901619824</v>
       </c>
-      <c r="F14">
-        <v>1.04849999999999</v>
-      </c>
       <c r="G14">
+        <v>-8.8134736994131102E-2</v>
+      </c>
+      <c r="H14">
+        <v>199.9</v>
+      </c>
+      <c r="I14">
+        <v>1282.5999999999999</v>
+      </c>
+      <c r="J14">
         <v>46</v>
       </c>
-      <c r="H14">
+      <c r="K14">
         <v>0.63393511114781698</v>
       </c>
-      <c r="I14">
+      <c r="L14">
+        <v>8.1314999999999298</v>
+      </c>
+      <c r="M14">
         <v>1.4591785525463599E-2</v>
       </c>
-      <c r="J14">
+      <c r="N14">
         <v>0.125522503998727</v>
       </c>
-      <c r="K14">
-        <v>8.1314999999999298</v>
-      </c>
-      <c r="L14">
+      <c r="O14">
+        <v>-0.110930718473263</v>
+      </c>
+      <c r="P14">
+        <v>386.4</v>
+      </c>
+      <c r="Q14">
+        <v>1522.5</v>
+      </c>
+      <c r="R14">
         <v>34.782608695652101</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>40</v>
       </c>
@@ -1693,34 +1995,52 @@
         <v>0.68211705231386099</v>
       </c>
       <c r="D15">
+        <v>7.3912499999999701</v>
+      </c>
+      <c r="E15">
         <v>1.9971619502526398E-2</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>0.22595442819525999</v>
       </c>
-      <c r="F15">
-        <v>7.3912499999999701</v>
-      </c>
       <c r="G15">
+        <v>-0.205982808692733</v>
+      </c>
+      <c r="H15">
+        <v>237.916666666666</v>
+      </c>
+      <c r="I15">
+        <v>1494.3333333333301</v>
+      </c>
+      <c r="J15">
         <v>46</v>
       </c>
-      <c r="H15">
+      <c r="K15">
         <v>0.52701962841759697</v>
       </c>
-      <c r="I15">
+      <c r="L15">
+        <v>10.53125</v>
+      </c>
+      <c r="M15">
         <v>1.3783077909267199E-2</v>
       </c>
-      <c r="J15">
+      <c r="N15">
         <v>0.11534160277135901</v>
       </c>
-      <c r="K15">
-        <v>10.53125</v>
-      </c>
-      <c r="L15">
+      <c r="O15">
+        <v>-0.10155852486209201</v>
+      </c>
+      <c r="P15">
+        <v>573.5</v>
+      </c>
+      <c r="Q15">
+        <v>1562.1666666666599</v>
+      </c>
+      <c r="R15">
         <v>30.434782608695599</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>40</v>
       </c>
@@ -1731,34 +2051,52 @@
         <v>0.84490863667545402</v>
       </c>
       <c r="D16">
+        <v>1.1766666666666601</v>
+      </c>
+      <c r="E16">
         <v>2.0138659789792498E-2</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>0.11114329192985101</v>
       </c>
-      <c r="F16">
-        <v>1.1766666666666601</v>
-      </c>
       <c r="G16">
+        <v>-9.1004632140058606E-2</v>
+      </c>
+      <c r="H16">
+        <v>172.444444444444</v>
+      </c>
+      <c r="I16">
+        <v>1319.55555555555</v>
+      </c>
+      <c r="J16">
         <v>46</v>
       </c>
-      <c r="H16">
+      <c r="K16">
         <v>0.70100535986421297</v>
       </c>
-      <c r="I16">
+      <c r="L16">
+        <v>6.2583333333332902</v>
+      </c>
+      <c r="M16">
         <v>1.84250830564467E-2</v>
       </c>
-      <c r="J16">
+      <c r="N16">
         <v>0.14727030392311699</v>
       </c>
-      <c r="K16">
-        <v>6.2583333333332902</v>
-      </c>
-      <c r="L16">
+      <c r="O16">
+        <v>-0.12884522086667</v>
+      </c>
+      <c r="P16">
+        <v>286.666666666666</v>
+      </c>
+      <c r="Q16">
+        <v>1458.55555555555</v>
+      </c>
+      <c r="R16">
         <v>21.739130434782599</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>40</v>
       </c>
@@ -1769,34 +2107,52 @@
         <v>0.71456948026414102</v>
       </c>
       <c r="D17">
+        <v>6.4462499999999503</v>
+      </c>
+      <c r="E17">
         <v>1.8990019969080198E-2</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>0.188419851925753</v>
       </c>
-      <c r="F17">
-        <v>6.4462499999999503</v>
-      </c>
       <c r="G17">
+        <v>-0.16942983195667299</v>
+      </c>
+      <c r="H17">
+        <v>277.83333333333297</v>
+      </c>
+      <c r="I17">
+        <v>1516.4166666666599</v>
+      </c>
+      <c r="J17">
         <v>47</v>
       </c>
-      <c r="H17">
+      <c r="K17">
         <v>0.53059351288510803</v>
       </c>
-      <c r="I17">
+      <c r="L17">
+        <v>10.414999999999999</v>
+      </c>
+      <c r="M17">
         <v>1.3805119862057E-2</v>
       </c>
-      <c r="J17">
+      <c r="N17">
         <v>0.10985488350573699</v>
       </c>
-      <c r="K17">
-        <v>10.414999999999999</v>
-      </c>
-      <c r="L17">
+      <c r="O17">
+        <v>-9.6049763643680397E-2</v>
+      </c>
+      <c r="P17">
+        <v>581.83333333333303</v>
+      </c>
+      <c r="Q17">
+        <v>1547.3333333333301</v>
+      </c>
+      <c r="R17">
         <v>34.042553191489297</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>40</v>
       </c>
@@ -1807,34 +2163,52 @@
         <v>0.84357776600577306</v>
       </c>
       <c r="D18">
+        <v>1.06499999999999</v>
+      </c>
+      <c r="E18">
         <v>2.2390571952855098E-2</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>0.111756261650276</v>
       </c>
-      <c r="F18">
-        <v>1.06499999999999</v>
-      </c>
       <c r="G18">
+        <v>-8.9365689697421202E-2</v>
+      </c>
+      <c r="H18">
+        <v>185.222222222222</v>
+      </c>
+      <c r="I18">
+        <v>1330.55555555555</v>
+      </c>
+      <c r="J18">
         <v>49</v>
       </c>
-      <c r="H18">
+      <c r="K18">
         <v>0.73999916958982803</v>
       </c>
-      <c r="I18">
+      <c r="L18">
+        <v>3.6983333333333199</v>
+      </c>
+      <c r="M18">
         <v>1.8231818536066299E-2</v>
       </c>
-      <c r="J18">
+      <c r="N18">
         <v>0.114063499050559</v>
       </c>
-      <c r="K18">
-        <v>3.6983333333333199</v>
-      </c>
-      <c r="L18">
+      <c r="O18">
+        <v>-9.5831680514493298E-2</v>
+      </c>
+      <c r="P18">
+        <v>405.33333333333297</v>
+      </c>
+      <c r="Q18">
+        <v>1246.3333333333301</v>
+      </c>
+      <c r="R18">
         <v>14.285714285714199</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>40</v>
       </c>
@@ -1845,34 +2219,52 @@
         <v>0.69307849509669905</v>
       </c>
       <c r="D19">
+        <v>7.6337500000000098</v>
+      </c>
+      <c r="E19">
         <v>1.8712943693313399E-2</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>0.228722365210345</v>
       </c>
-      <c r="F19">
-        <v>7.6337500000000098</v>
-      </c>
       <c r="G19">
+        <v>-0.210009421517032</v>
+      </c>
+      <c r="H19">
+        <v>197.75</v>
+      </c>
+      <c r="I19">
+        <v>1582.1666666666599</v>
+      </c>
+      <c r="J19">
         <v>46</v>
       </c>
-      <c r="H19">
+      <c r="K19">
         <v>0.52821223408399298</v>
       </c>
-      <c r="I19">
+      <c r="L19">
+        <v>10.463749999999999</v>
+      </c>
+      <c r="M19">
         <v>1.41337762541065E-2</v>
       </c>
-      <c r="J19">
+      <c r="N19">
         <v>0.112569663899394</v>
       </c>
-      <c r="K19">
-        <v>10.463749999999999</v>
-      </c>
-      <c r="L19">
+      <c r="O19">
+        <v>-9.8435887645287601E-2</v>
+      </c>
+      <c r="P19">
+        <v>598.25</v>
+      </c>
+      <c r="Q19">
+        <v>1546.0833333333301</v>
+      </c>
+      <c r="R19">
         <v>32.6086956521739</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>40</v>
       </c>
@@ -1883,34 +2275,52 @@
         <v>0.77025462061813998</v>
       </c>
       <c r="D20">
+        <v>3.7990909090909</v>
+      </c>
+      <c r="E20">
         <v>2.2006283664658299E-2</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>0.17224022688695201</v>
       </c>
-      <c r="F20">
-        <v>3.7990909090909</v>
-      </c>
       <c r="G20">
+        <v>-0.150233943222293</v>
+      </c>
+      <c r="H20">
+        <v>202.72727272727201</v>
+      </c>
+      <c r="I20">
+        <v>1452.0909090908999</v>
+      </c>
+      <c r="J20">
         <v>46</v>
       </c>
-      <c r="H20">
+      <c r="K20">
         <v>0.57890827413997004</v>
       </c>
-      <c r="I20">
+      <c r="L20">
+        <v>9.0640909090908703</v>
+      </c>
+      <c r="M20">
         <v>1.4461888107220501E-2</v>
       </c>
-      <c r="J20">
+      <c r="N20">
         <v>0.11496378371745899</v>
       </c>
-      <c r="K20">
-        <v>9.0640909090908703</v>
-      </c>
-      <c r="L20">
+      <c r="O20">
+        <v>-0.10050189561023801</v>
+      </c>
+      <c r="P20">
+        <v>520.45454545454504</v>
+      </c>
+      <c r="Q20">
+        <v>1530</v>
+      </c>
+      <c r="R20">
         <v>34.782608695652101</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>40</v>
       </c>
@@ -1921,34 +2331,52 @@
         <v>0.70094872402730601</v>
       </c>
       <c r="D21">
+        <v>7.4499999999999602</v>
+      </c>
+      <c r="E21">
         <v>1.8972006132383399E-2</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>0.24736535033538501</v>
       </c>
-      <c r="F21">
-        <v>7.4499999999999602</v>
-      </c>
       <c r="G21">
+        <v>-0.228393344203002</v>
+      </c>
+      <c r="H21">
+        <v>167.083333333333</v>
+      </c>
+      <c r="I21">
+        <v>1553.4166666666599</v>
+      </c>
+      <c r="J21">
         <v>46</v>
       </c>
-      <c r="H21">
+      <c r="K21">
         <v>0.52715903970568001</v>
       </c>
-      <c r="I21">
+      <c r="L21">
+        <v>9.9537499999999905</v>
+      </c>
+      <c r="M21">
         <v>1.3661632515368701E-2</v>
       </c>
-      <c r="J21">
+      <c r="N21">
         <v>0.107036747075316</v>
       </c>
-      <c r="K21">
-        <v>9.9537499999999905</v>
-      </c>
-      <c r="L21">
+      <c r="O21">
+        <v>-9.3375114559947597E-2</v>
+      </c>
+      <c r="P21">
+        <v>671.08333333333303</v>
+      </c>
+      <c r="Q21">
+        <v>1509</v>
+      </c>
+      <c r="R21">
         <v>34.782608695652101</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>40</v>
       </c>
@@ -1959,34 +2387,52 @@
         <v>0.66877072930822201</v>
       </c>
       <c r="D22">
+        <v>7.7424999999999997</v>
+      </c>
+      <c r="E22">
         <v>2.07419753509256E-2</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>0.236439952433945</v>
       </c>
-      <c r="F22">
-        <v>7.7424999999999997</v>
-      </c>
       <c r="G22">
+        <v>-0.21569797708301899</v>
+      </c>
+      <c r="H22">
+        <v>255.916666666666</v>
+      </c>
+      <c r="I22">
+        <v>1544.5833333333301</v>
+      </c>
+      <c r="J22">
         <v>46</v>
       </c>
-      <c r="H22">
+      <c r="K22">
         <v>0.52957987178830201</v>
       </c>
-      <c r="I22">
+      <c r="L22">
+        <v>10.421250000000001</v>
+      </c>
+      <c r="M22">
         <v>1.38105046818634E-2</v>
       </c>
-      <c r="J22">
+      <c r="N22">
         <v>0.11472314091526201</v>
       </c>
-      <c r="K22">
-        <v>10.421250000000001</v>
-      </c>
-      <c r="L22">
+      <c r="O22">
+        <v>-0.10091263623339899</v>
+      </c>
+      <c r="P22">
+        <v>587.16666666666595</v>
+      </c>
+      <c r="Q22">
+        <v>1550.0833333333301</v>
+      </c>
+      <c r="R22">
         <v>28.260869565217298</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>40</v>
       </c>
@@ -1997,34 +2443,52 @@
         <v>0.64867568814447796</v>
       </c>
       <c r="D23">
+        <v>9.0749999999999797</v>
+      </c>
+      <c r="E23">
         <v>2.3279900128129399E-2</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>0.27221931794485399</v>
       </c>
-      <c r="F23">
-        <v>9.0749999999999797</v>
-      </c>
       <c r="G23">
+        <v>-0.24893941781672499</v>
+      </c>
+      <c r="H23">
+        <v>230.230769230769</v>
+      </c>
+      <c r="I23">
+        <v>1622.8461538461499</v>
+      </c>
+      <c r="J23">
         <v>47</v>
       </c>
-      <c r="H23">
+      <c r="K23">
         <v>0.49023072866464301</v>
       </c>
-      <c r="I23">
+      <c r="L23">
+        <v>10.899230769230799</v>
+      </c>
+      <c r="M23">
         <v>1.3510568948839501E-2</v>
       </c>
-      <c r="J23">
+      <c r="N23">
         <v>9.9050218797378103E-2</v>
       </c>
-      <c r="K23">
-        <v>10.899230769230799</v>
-      </c>
-      <c r="L23">
+      <c r="O23">
+        <v>-8.5539649848538499E-2</v>
+      </c>
+      <c r="P23">
+        <v>726.461538461538</v>
+      </c>
+      <c r="Q23">
+        <v>1521.38461538461</v>
+      </c>
+      <c r="R23">
         <v>31.9148936170212</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>40</v>
       </c>
@@ -2035,34 +2499,52 @@
         <v>0.74785592451267502</v>
       </c>
       <c r="D24">
+        <v>4.9118181818181599</v>
+      </c>
+      <c r="E24">
         <v>1.8357781679465199E-2</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>0.18393849610430299</v>
       </c>
-      <c r="F24">
-        <v>4.9118181818181599</v>
-      </c>
       <c r="G24">
+        <v>-0.16558071442483699</v>
+      </c>
+      <c r="H24">
+        <v>215.54545454545399</v>
+      </c>
+      <c r="I24">
+        <v>1481.8181818181799</v>
+      </c>
+      <c r="J24">
         <v>46</v>
       </c>
-      <c r="H24">
+      <c r="K24">
         <v>0.56877399363896997</v>
       </c>
-      <c r="I24">
+      <c r="L24">
+        <v>9.3504545454545198</v>
+      </c>
+      <c r="M24">
         <v>1.4483308340271599E-2</v>
       </c>
-      <c r="J24">
+      <c r="N24">
         <v>0.117170357678725</v>
       </c>
-      <c r="K24">
-        <v>9.3504545454545198</v>
-      </c>
-      <c r="L24">
+      <c r="O24">
+        <v>-0.102687049338454</v>
+      </c>
+      <c r="P24">
+        <v>542.54545454545405</v>
+      </c>
+      <c r="Q24">
+        <v>1531</v>
+      </c>
+      <c r="R24">
         <v>32.6086956521739</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>40</v>
       </c>
@@ -2073,34 +2555,52 @@
         <v>0.775070671321058</v>
       </c>
       <c r="D25">
+        <v>3.8918181818181701</v>
+      </c>
+      <c r="E25">
         <v>2.057004442091E-2</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>0.17064274519185799</v>
       </c>
-      <c r="F25">
-        <v>3.8918181818181701</v>
-      </c>
       <c r="G25">
+        <v>-0.150072700770948</v>
+      </c>
+      <c r="H25">
+        <v>206.363636363636</v>
+      </c>
+      <c r="I25">
+        <v>1459.54545454545</v>
+      </c>
+      <c r="J25">
         <v>46</v>
       </c>
-      <c r="H25">
+      <c r="K25">
         <v>0.58413158478417104</v>
       </c>
-      <c r="I25">
+      <c r="L25">
+        <v>8.9168181818181402</v>
+      </c>
+      <c r="M25">
         <v>1.39829657959878E-2</v>
       </c>
-      <c r="J25">
+      <c r="N25">
         <v>0.11517146548516601</v>
       </c>
-      <c r="K25">
-        <v>8.9168181818181402</v>
-      </c>
-      <c r="L25">
+      <c r="O25">
+        <v>-0.10118849968917799</v>
+      </c>
+      <c r="P25">
+        <v>532</v>
+      </c>
+      <c r="Q25">
+        <v>1502.3636363636299</v>
+      </c>
+      <c r="R25">
         <v>34.782608695652101</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>40</v>
       </c>
@@ -2111,34 +2611,52 @@
         <v>0.70090176448931896</v>
       </c>
       <c r="D26">
+        <v>7.8612499999999503</v>
+      </c>
+      <c r="E26">
         <v>1.8387795545535501E-2</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>0.246036446860043</v>
       </c>
-      <c r="F26">
-        <v>7.8612499999999503</v>
-      </c>
       <c r="G26">
+        <v>-0.22764865131450701</v>
+      </c>
+      <c r="H26">
+        <v>165.75</v>
+      </c>
+      <c r="I26">
+        <v>1582.5</v>
+      </c>
+      <c r="J26">
         <v>46</v>
       </c>
-      <c r="H26">
+      <c r="K26">
         <v>0.53272342698399799</v>
       </c>
-      <c r="I26">
+      <c r="L26">
+        <v>9.8374999999999897</v>
+      </c>
+      <c r="M26">
         <v>1.3439200962326399E-2</v>
       </c>
-      <c r="J26">
+      <c r="N26">
         <v>0.10662296721556699</v>
       </c>
-      <c r="K26">
-        <v>9.8374999999999897</v>
-      </c>
-      <c r="L26">
+      <c r="O26">
+        <v>-9.3183766253241193E-2</v>
+      </c>
+      <c r="P26">
+        <v>656.83333333333303</v>
+      </c>
+      <c r="Q26">
+        <v>1506.4166666666599</v>
+      </c>
+      <c r="R26">
         <v>32.6086956521739</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>40</v>
       </c>
@@ -2149,34 +2667,52 @@
         <v>0.75396897757575199</v>
       </c>
       <c r="D27">
+        <v>4.6472727272727097</v>
+      </c>
+      <c r="E27">
         <v>1.90829951523954E-2</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>0.179004096472133</v>
       </c>
-      <c r="F27">
-        <v>4.6472727272727097</v>
-      </c>
       <c r="G27">
+        <v>-0.159921101319738</v>
+      </c>
+      <c r="H27">
+        <v>210.636363636363</v>
+      </c>
+      <c r="I27">
+        <v>1480.9090909090901</v>
+      </c>
+      <c r="J27">
         <v>46</v>
       </c>
-      <c r="H27">
+      <c r="K27">
         <v>0.58380473147613998</v>
       </c>
-      <c r="I27">
+      <c r="L27">
+        <v>8.9331818181817795</v>
+      </c>
+      <c r="M27">
         <v>1.4305638617244701E-2</v>
       </c>
-      <c r="J27">
+      <c r="N27">
         <v>0.11612420652812799</v>
       </c>
-      <c r="K27">
-        <v>8.9331818181817795</v>
-      </c>
-      <c r="L27">
+      <c r="O27">
+        <v>-0.10181856791088301</v>
+      </c>
+      <c r="P27">
+        <v>518</v>
+      </c>
+      <c r="Q27">
+        <v>1513.27272727272</v>
+      </c>
+      <c r="R27">
         <v>32.6086956521739</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>40</v>
       </c>
@@ -2187,34 +2723,52 @@
         <v>0.75083520400991199</v>
       </c>
       <c r="D28">
+        <v>5.2540909090908903</v>
+      </c>
+      <c r="E28">
         <v>1.7459227482497099E-2</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>0.19886356007286701</v>
       </c>
-      <c r="F28">
-        <v>5.2540909090908903</v>
-      </c>
       <c r="G28">
+        <v>-0.18140433259037</v>
+      </c>
+      <c r="H28">
+        <v>178.18181818181799</v>
+      </c>
+      <c r="I28">
+        <v>1499.1818181818101</v>
+      </c>
+      <c r="J28">
         <v>45</v>
       </c>
-      <c r="H28">
+      <c r="K28">
         <v>0.58082881919447604</v>
       </c>
-      <c r="I28">
+      <c r="L28">
+        <v>9.0122727272726895</v>
+      </c>
+      <c r="M28">
         <v>1.3930198648627899E-2</v>
       </c>
-      <c r="J28">
+      <c r="N28">
         <v>0.11958215014832201</v>
       </c>
-      <c r="K28">
-        <v>9.0122727272726895</v>
-      </c>
-      <c r="L28">
+      <c r="O28">
+        <v>-0.105651951499694</v>
+      </c>
+      <c r="P28">
+        <v>523.63636363636294</v>
+      </c>
+      <c r="Q28">
+        <v>1510.3636363636299</v>
+      </c>
+      <c r="R28">
         <v>31.1111111111111</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>40</v>
       </c>
@@ -2225,34 +2779,52 @@
         <v>0.851610977048878</v>
       </c>
       <c r="D29">
+        <v>1.1033333333333299</v>
+      </c>
+      <c r="E29">
         <v>1.86096913872912E-2</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>0.112017135575065</v>
       </c>
-      <c r="F29">
-        <v>1.1033333333333299</v>
-      </c>
       <c r="G29">
+        <v>-9.3407444187774594E-2</v>
+      </c>
+      <c r="H29">
+        <v>159.777777777777</v>
+      </c>
+      <c r="I29">
+        <v>1314.88888888888</v>
+      </c>
+      <c r="J29">
         <v>46</v>
       </c>
-      <c r="H29">
+      <c r="K29">
         <v>0.70235673097428097</v>
       </c>
-      <c r="I29">
+      <c r="L29">
+        <v>6.2533333333332903</v>
+      </c>
+      <c r="M29">
         <v>1.71568034231089E-2</v>
       </c>
-      <c r="J29">
+      <c r="N29">
         <v>0.14565761467889099</v>
       </c>
-      <c r="K29">
-        <v>6.2533333333332903</v>
-      </c>
-      <c r="L29">
+      <c r="O29">
+        <v>-0.128500811255782</v>
+      </c>
+      <c r="P29">
+        <v>284.77777777777698</v>
+      </c>
+      <c r="Q29">
+        <v>1452.44444444444</v>
+      </c>
+      <c r="R29">
         <v>23.9130434782608</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>40</v>
       </c>
@@ -2263,34 +2835,52 @@
         <v>0.64240690598866002</v>
       </c>
       <c r="D30">
+        <v>9.5642307692307504</v>
+      </c>
+      <c r="E30">
         <v>2.2869251422327399E-2</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>0.27944320489560098</v>
       </c>
-      <c r="F30">
-        <v>9.5642307692307504</v>
-      </c>
       <c r="G30">
+        <v>-0.256573953473273</v>
+      </c>
+      <c r="H30">
+        <v>232</v>
+      </c>
+      <c r="I30">
+        <v>1651.4615384615299</v>
+      </c>
+      <c r="J30">
         <v>46</v>
       </c>
-      <c r="H30">
+      <c r="K30">
         <v>0.48639272280201301</v>
       </c>
-      <c r="I30">
+      <c r="L30">
+        <v>11.1426923076923</v>
+      </c>
+      <c r="M30">
         <v>1.34958585417446E-2</v>
       </c>
-      <c r="J30">
+      <c r="N30">
         <v>0.106941628437838</v>
       </c>
-      <c r="K30">
-        <v>11.1426923076923</v>
-      </c>
-      <c r="L30">
+      <c r="O30">
+        <v>-9.3445769896093503E-2</v>
+      </c>
+      <c r="P30">
+        <v>713.07692307692298</v>
+      </c>
+      <c r="Q30">
+        <v>1535.6923076922999</v>
+      </c>
+      <c r="R30">
         <v>34.782608695652101</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>40</v>
       </c>
@@ -2301,34 +2891,52 @@
         <v>0.62134820615879505</v>
       </c>
       <c r="D31">
+        <v>9.3392307692307508</v>
+      </c>
+      <c r="E31">
         <v>2.7240737854176501E-2</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>0.45196074999887997</v>
       </c>
-      <c r="F31">
-        <v>9.3392307692307508</v>
-      </c>
       <c r="G31">
+        <v>-0.42472001214470401</v>
+      </c>
+      <c r="H31">
+        <v>285.923076923076</v>
+      </c>
+      <c r="I31">
+        <v>1635.38461538461</v>
+      </c>
+      <c r="J31">
         <v>46</v>
       </c>
-      <c r="H31">
+      <c r="K31">
         <v>0.48692923825531897</v>
       </c>
-      <c r="I31">
+      <c r="L31">
+        <v>10.8842307692308</v>
+      </c>
+      <c r="M31">
         <v>1.3074666624689601E-2</v>
       </c>
-      <c r="J31">
+      <c r="N31">
         <v>0.13924547735637599</v>
       </c>
-      <c r="K31">
-        <v>10.8842307692308</v>
-      </c>
-      <c r="L31">
+      <c r="O31">
+        <v>-0.12617081073168601</v>
+      </c>
+      <c r="P31">
+        <v>725.15384615384596</v>
+      </c>
+      <c r="Q31">
+        <v>1540.4615384615299</v>
+      </c>
+      <c r="R31">
         <v>28.260869565217298</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>40</v>
       </c>
@@ -2339,34 +2947,52 @@
         <v>0.84155358272800596</v>
       </c>
       <c r="D32">
+        <v>1.12949999999999</v>
+      </c>
+      <c r="E32">
         <v>2.11918870537047E-2</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>0.11427220885851901</v>
       </c>
-      <c r="F32">
-        <v>1.12949999999999</v>
-      </c>
       <c r="G32">
+        <v>-9.3080321804814403E-2</v>
+      </c>
+      <c r="H32">
+        <v>197.8</v>
+      </c>
+      <c r="I32">
+        <v>1345.6</v>
+      </c>
+      <c r="J32">
         <v>46</v>
       </c>
-      <c r="H32">
+      <c r="K32">
         <v>0.63016179851133203</v>
       </c>
-      <c r="I32">
+      <c r="L32">
+        <v>7.6950000000000003</v>
+      </c>
+      <c r="M32">
         <v>1.6343070468092601E-2</v>
       </c>
-      <c r="J32">
+      <c r="N32">
         <v>0.13662936565756501</v>
       </c>
-      <c r="K32">
-        <v>7.6950000000000003</v>
-      </c>
-      <c r="L32">
+      <c r="O32">
+        <v>-0.12028629518947299</v>
+      </c>
+      <c r="P32">
+        <v>445.8</v>
+      </c>
+      <c r="Q32">
+        <v>1461.7</v>
+      </c>
+      <c r="R32">
         <v>36.956521739130402</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>40</v>
       </c>
@@ -2377,34 +3003,52 @@
         <v>0.69928331412845002</v>
       </c>
       <c r="D33">
+        <v>7.5974999999999397</v>
+      </c>
+      <c r="E33">
         <v>1.85658825971282E-2</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>0.24534134120201001</v>
       </c>
-      <c r="F33">
-        <v>7.5974999999999397</v>
-      </c>
       <c r="G33">
+        <v>-0.22677545860488199</v>
+      </c>
+      <c r="H33">
+        <v>174.666666666666</v>
+      </c>
+      <c r="I33">
+        <v>1561.0833333333301</v>
+      </c>
+      <c r="J33">
         <v>46</v>
       </c>
-      <c r="H33">
+      <c r="K33">
         <v>0.53164989037826005</v>
       </c>
-      <c r="I33">
+      <c r="L33">
+        <v>9.8737499999999905</v>
+      </c>
+      <c r="M33">
         <v>1.37085081325788E-2</v>
       </c>
-      <c r="J33">
+      <c r="N33">
         <v>0.108633566838252</v>
       </c>
-      <c r="K33">
-        <v>9.8737499999999905</v>
-      </c>
-      <c r="L33">
+      <c r="O33">
+        <v>-9.4925058705673707E-2</v>
+      </c>
+      <c r="P33">
+        <v>663.75</v>
+      </c>
+      <c r="Q33">
+        <v>1505.6666666666599</v>
+      </c>
+      <c r="R33">
         <v>32.6086956521739</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>40</v>
       </c>
@@ -2415,34 +3059,52 @@
         <v>0.68599872034086395</v>
       </c>
       <c r="D34">
+        <v>7.3037499999999804</v>
+      </c>
+      <c r="E34">
         <v>1.97834751065082E-2</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>0.22256823875033099</v>
       </c>
-      <c r="F34">
-        <v>7.3037499999999804</v>
-      </c>
       <c r="G34">
+        <v>-0.202784763643823</v>
+      </c>
+      <c r="H34">
+        <v>240.166666666666</v>
+      </c>
+      <c r="I34">
+        <v>1495.0833333333301</v>
+      </c>
+      <c r="J34">
         <v>46</v>
       </c>
-      <c r="H34">
+      <c r="K34">
         <v>0.52828982222789</v>
       </c>
-      <c r="I34">
+      <c r="L34">
+        <v>10.445</v>
+      </c>
+      <c r="M34">
         <v>1.3929311625294E-2</v>
       </c>
-      <c r="J34">
+      <c r="N34">
         <v>0.109560633379859</v>
       </c>
-      <c r="K34">
-        <v>10.445</v>
-      </c>
-      <c r="L34">
+      <c r="O34">
+        <v>-9.5631321754565499E-2</v>
+      </c>
+      <c r="P34">
+        <v>581.5</v>
+      </c>
+      <c r="Q34">
+        <v>1563</v>
+      </c>
+      <c r="R34">
         <v>30.434782608695599</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>40</v>
       </c>
@@ -2453,34 +3115,52 @@
         <v>0.79528969454236298</v>
       </c>
       <c r="D35">
+        <v>3.23999999999999</v>
+      </c>
+      <c r="E35">
         <v>1.7210378751476199E-2</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>0.145795981626025</v>
       </c>
-      <c r="F35">
-        <v>3.23999999999999</v>
-      </c>
       <c r="G35">
+        <v>-0.12858560287454801</v>
+      </c>
+      <c r="H35">
+        <v>195.4</v>
+      </c>
+      <c r="I35">
+        <v>1317</v>
+      </c>
+      <c r="J35">
         <v>46</v>
       </c>
-      <c r="H35">
+      <c r="K35">
         <v>0.63326749620078404</v>
       </c>
-      <c r="I35">
+      <c r="L35">
+        <v>8.1344999999999299</v>
+      </c>
+      <c r="M35">
         <v>1.4894852742515801E-2</v>
       </c>
-      <c r="J35">
+      <c r="N35">
         <v>0.12806349971278999</v>
       </c>
-      <c r="K35">
-        <v>8.1344999999999299</v>
-      </c>
-      <c r="L35">
+      <c r="O35">
+        <v>-0.113168646970274</v>
+      </c>
+      <c r="P35">
+        <v>386.9</v>
+      </c>
+      <c r="Q35">
+        <v>1532.2</v>
+      </c>
+      <c r="R35">
         <v>26.086956521739101</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>40</v>
       </c>
@@ -2491,34 +3171,52 @@
         <v>0.64856762760256703</v>
       </c>
       <c r="D36">
+        <v>9.3669230769230492</v>
+      </c>
+      <c r="E36">
         <v>2.17790547157246E-2</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>0.27446496563610601</v>
       </c>
-      <c r="F36">
-        <v>9.3669230769230492</v>
-      </c>
       <c r="G36">
+        <v>-0.25268591092038101</v>
+      </c>
+      <c r="H36">
+        <v>225.76923076923001</v>
+      </c>
+      <c r="I36">
+        <v>1638.76923076923</v>
+      </c>
+      <c r="J36">
         <v>46</v>
       </c>
-      <c r="H36">
+      <c r="K36">
         <v>0.486111041559048</v>
       </c>
-      <c r="I36">
+      <c r="L36">
+        <v>11.125384615384601</v>
+      </c>
+      <c r="M36">
         <v>1.34874022036593E-2</v>
       </c>
-      <c r="J36">
+      <c r="N36">
         <v>0.1012871632728</v>
       </c>
-      <c r="K36">
-        <v>11.125384615384601</v>
-      </c>
-      <c r="L36">
+      <c r="O36">
+        <v>-8.7799761069140905E-2</v>
+      </c>
+      <c r="P36">
+        <v>722.461538461538</v>
+      </c>
+      <c r="Q36">
+        <v>1529.76923076923</v>
+      </c>
+      <c r="R36">
         <v>34.782608695652101</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>40</v>
       </c>
@@ -2529,34 +3227,52 @@
         <v>0.80422235148524801</v>
       </c>
       <c r="D37">
+        <v>2.8319999999999999</v>
+      </c>
+      <c r="E37">
         <v>1.5279838285164601E-2</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>0.15107416482739</v>
       </c>
-      <c r="F37">
-        <v>2.8319999999999999</v>
-      </c>
       <c r="G37">
+        <v>-0.13579432654222501</v>
+      </c>
+      <c r="H37">
+        <v>185.4</v>
+      </c>
+      <c r="I37">
+        <v>1430.7</v>
+      </c>
+      <c r="J37">
         <v>46</v>
       </c>
-      <c r="H37">
+      <c r="K37">
         <v>0.63055295347337004</v>
       </c>
-      <c r="I37">
+      <c r="L37">
+        <v>8.1689999999999401</v>
+      </c>
+      <c r="M37">
         <v>1.47862156204316E-2</v>
       </c>
-      <c r="J37">
+      <c r="N37">
         <v>0.12479201823898101</v>
       </c>
-      <c r="K37">
-        <v>8.1689999999999401</v>
-      </c>
-      <c r="L37">
+      <c r="O37">
+        <v>-0.110005802618549</v>
+      </c>
+      <c r="P37">
+        <v>386.5</v>
+      </c>
+      <c r="Q37">
+        <v>1531.9</v>
+      </c>
+      <c r="R37">
         <v>30.434782608695599</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>40</v>
       </c>
@@ -2567,34 +3283,52 @@
         <v>0.65468732510393701</v>
       </c>
       <c r="D38">
+        <v>8.9053846153845893</v>
+      </c>
+      <c r="E38">
         <v>2.2756567947308501E-2</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>0.27031349646317399</v>
       </c>
-      <c r="F38">
-        <v>8.9053846153845893</v>
-      </c>
       <c r="G38">
+        <v>-0.247556928515866</v>
+      </c>
+      <c r="H38">
+        <v>220.76923076923001</v>
+      </c>
+      <c r="I38">
+        <v>1607.9230769230701</v>
+      </c>
+      <c r="J38">
         <v>46</v>
       </c>
-      <c r="H38">
+      <c r="K38">
         <v>0.49131766637445801</v>
       </c>
-      <c r="I38">
+      <c r="L38">
+        <v>11.0723076923077</v>
+      </c>
+      <c r="M38">
         <v>1.36248273911195E-2</v>
       </c>
-      <c r="J38">
+      <c r="N38">
         <v>0.105506906533732</v>
       </c>
-      <c r="K38">
-        <v>11.0723076923077</v>
-      </c>
-      <c r="L38">
+      <c r="O38">
+        <v>-9.1882079142612705E-2</v>
+      </c>
+      <c r="P38">
+        <v>704.69230769230705</v>
+      </c>
+      <c r="Q38">
+        <v>1526.23076923076</v>
+      </c>
+      <c r="R38">
         <v>34.782608695652101</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>40</v>
       </c>
@@ -2605,34 +3339,52 @@
         <v>0.69289817132501097</v>
       </c>
       <c r="D39">
+        <v>7.4024999999999901</v>
+      </c>
+      <c r="E39">
         <v>1.9821531999057701E-2</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>0.23165519145963701</v>
       </c>
-      <c r="F39">
-        <v>7.4024999999999901</v>
-      </c>
       <c r="G39">
+        <v>-0.21183365946058</v>
+      </c>
+      <c r="H39">
+        <v>197.75</v>
+      </c>
+      <c r="I39">
+        <v>1566</v>
+      </c>
+      <c r="J39">
         <v>47</v>
       </c>
-      <c r="H39">
+      <c r="K39">
         <v>0.53004690551789901</v>
       </c>
-      <c r="I39">
+      <c r="L39">
+        <v>10.39</v>
+      </c>
+      <c r="M39">
         <v>1.3957803362640299E-2</v>
       </c>
-      <c r="J39">
+      <c r="N39">
         <v>0.11064658750186999</v>
       </c>
-      <c r="K39">
-        <v>10.39</v>
-      </c>
-      <c r="L39">
+      <c r="O39">
+        <v>-9.6688784139230197E-2</v>
+      </c>
+      <c r="P39">
+        <v>597.58333333333303</v>
+      </c>
+      <c r="Q39">
+        <v>1545.25</v>
+      </c>
+      <c r="R39">
         <v>29.787234042553099</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>40</v>
       </c>
@@ -2643,34 +3395,52 @@
         <v>0.84504729259282596</v>
       </c>
       <c r="D40">
+        <v>1.2389999999999901</v>
+      </c>
+      <c r="E40">
         <v>2.0697043729014999E-2</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>0.11190324815649599</v>
       </c>
-      <c r="F40">
-        <v>1.2389999999999901</v>
-      </c>
       <c r="G40">
+        <v>-9.1206204427480994E-2</v>
+      </c>
+      <c r="H40">
+        <v>191.4</v>
+      </c>
+      <c r="I40">
+        <v>1320.4</v>
+      </c>
+      <c r="J40">
         <v>46</v>
       </c>
-      <c r="H40">
+      <c r="K40">
         <v>0.63671869627532995</v>
       </c>
-      <c r="I40">
+      <c r="L40">
+        <v>7.4099999999999904</v>
+      </c>
+      <c r="M40">
         <v>1.60624479129561E-2</v>
       </c>
-      <c r="J40">
+      <c r="N40">
         <v>0.13260563322886501</v>
       </c>
-      <c r="K40">
-        <v>7.4099999999999904</v>
-      </c>
-      <c r="L40">
+      <c r="O40">
+        <v>-0.116543185315909</v>
+      </c>
+      <c r="P40">
+        <v>450</v>
+      </c>
+      <c r="Q40">
+        <v>1451.2</v>
+      </c>
+      <c r="R40">
         <v>34.782608695652101</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2681,34 +3451,52 @@
         <v>0.70606885353337601</v>
       </c>
       <c r="D41">
+        <v>7.4649999999999501</v>
+      </c>
+      <c r="E41">
         <v>1.8284886398068599E-2</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>0.24254309514011499</v>
       </c>
-      <c r="F41">
-        <v>7.4649999999999501</v>
-      </c>
       <c r="G41">
+        <v>-0.22425820874204599</v>
+      </c>
+      <c r="H41">
+        <v>160.25</v>
+      </c>
+      <c r="I41">
+        <v>1543.3333333333301</v>
+      </c>
+      <c r="J41">
         <v>46</v>
       </c>
-      <c r="H41">
+      <c r="K41">
         <v>0.53913730118744396</v>
       </c>
-      <c r="I41">
+      <c r="L41">
+        <v>9.6187499999999808</v>
+      </c>
+      <c r="M41">
         <v>1.35695839408206E-2</v>
       </c>
-      <c r="J41">
+      <c r="N41">
         <v>0.106794066732747</v>
       </c>
-      <c r="K41">
-        <v>9.6187499999999808</v>
-      </c>
-      <c r="L41">
+      <c r="O41">
+        <v>-9.3224482791926605E-2</v>
+      </c>
+      <c r="P41">
+        <v>650.5</v>
+      </c>
+      <c r="Q41">
+        <v>1496.25</v>
+      </c>
+      <c r="R41">
         <v>32.6086956521739</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2719,34 +3507,52 @@
         <v>0.82336099668157603</v>
       </c>
       <c r="D42">
+        <v>1.9649999999999901</v>
+      </c>
+      <c r="E42">
         <v>2.42667080210551E-2</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>0.12550614548772299</v>
       </c>
-      <c r="F42">
-        <v>1.9649999999999901</v>
-      </c>
       <c r="G42">
+        <v>-0.101239437466668</v>
+      </c>
+      <c r="H42">
+        <v>215.5</v>
+      </c>
+      <c r="I42">
+        <v>1302.0999999999999</v>
+      </c>
+      <c r="J42">
         <v>48</v>
       </c>
-      <c r="H42">
+      <c r="K42">
         <v>0.66635791952420897</v>
       </c>
-      <c r="I42">
+      <c r="L42">
+        <v>5.9024999999999501</v>
+      </c>
+      <c r="M42">
         <v>1.6331542845400299E-2</v>
       </c>
-      <c r="J42">
+      <c r="N42">
         <v>0.124355106960754</v>
       </c>
-      <c r="K42">
-        <v>5.9024999999999501</v>
-      </c>
-      <c r="L42">
+      <c r="O42">
+        <v>-0.10802356411535401</v>
+      </c>
+      <c r="P42">
+        <v>498.8</v>
+      </c>
+      <c r="Q42">
+        <v>1290.3</v>
+      </c>
+      <c r="R42">
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>40</v>
       </c>
@@ -2757,34 +3563,52 @@
         <v>0.649254769610765</v>
       </c>
       <c r="D43">
+        <v>9.23192307692306</v>
+      </c>
+      <c r="E43">
         <v>2.24824182711248E-2</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>0.27310152498511198</v>
       </c>
-      <c r="F43">
-        <v>9.23192307692306</v>
-      </c>
       <c r="G43">
+        <v>-0.25061910671398702</v>
+      </c>
+      <c r="H43">
+        <v>224.38461538461499</v>
+      </c>
+      <c r="I43">
+        <v>1629.76923076923</v>
+      </c>
+      <c r="J43">
         <v>46</v>
       </c>
-      <c r="H43">
+      <c r="K43">
         <v>0.48894222871864301</v>
       </c>
-      <c r="I43">
+      <c r="L43">
+        <v>11.0826923076923</v>
+      </c>
+      <c r="M43">
         <v>1.35210598981751E-2</v>
       </c>
-      <c r="J43">
+      <c r="N43">
         <v>0.10317719568577099</v>
       </c>
-      <c r="K43">
-        <v>11.0826923076923</v>
-      </c>
-      <c r="L43">
+      <c r="O43">
+        <v>-8.9656135787596306E-2</v>
+      </c>
+      <c r="P43">
+        <v>714.07692307692298</v>
+      </c>
+      <c r="Q43">
+        <v>1531.23076923076</v>
+      </c>
+      <c r="R43">
         <v>34.782608695652101</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>40</v>
       </c>
@@ -2795,34 +3619,52 @@
         <v>0.76836244256335895</v>
       </c>
       <c r="D44">
+        <v>4.1659090909090803</v>
+      </c>
+      <c r="E44">
         <v>2.0435580407158298E-2</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>0.161054482935796</v>
       </c>
-      <c r="F44">
-        <v>4.1659090909090803</v>
-      </c>
       <c r="G44">
+        <v>-0.14061890252863701</v>
+      </c>
+      <c r="H44">
+        <v>227.45454545454501</v>
+      </c>
+      <c r="I44">
+        <v>1277.9090909090901</v>
+      </c>
+      <c r="J44">
         <v>46</v>
       </c>
-      <c r="H44">
+      <c r="K44">
         <v>0.58276766527009205</v>
       </c>
-      <c r="I44">
+      <c r="L44">
+        <v>8.9604545454545796</v>
+      </c>
+      <c r="M44">
         <v>1.5554015317215401E-2</v>
       </c>
-      <c r="J44">
+      <c r="N44">
         <v>0.12648042028308601</v>
       </c>
-      <c r="K44">
-        <v>8.9604545454545796</v>
-      </c>
-      <c r="L44">
+      <c r="O44">
+        <v>-0.11092640496587</v>
+      </c>
+      <c r="P44">
+        <v>517.27272727272702</v>
+      </c>
+      <c r="Q44">
+        <v>1469.8181818181799</v>
+      </c>
+      <c r="R44">
         <v>34.782608695652101</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>40</v>
       </c>
@@ -2833,34 +3675,52 @@
         <v>0.82641639902778097</v>
       </c>
       <c r="D45">
+        <v>1.94549999999999</v>
+      </c>
+      <c r="E45">
         <v>1.9920819499038601E-2</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>3.0218851474114898</v>
       </c>
-      <c r="F45">
-        <v>1.94549999999999</v>
-      </c>
       <c r="G45">
+        <v>-3.0019643279124502</v>
+      </c>
+      <c r="H45">
+        <v>190.6</v>
+      </c>
+      <c r="I45">
+        <v>1364.7</v>
+      </c>
+      <c r="J45">
         <v>45</v>
       </c>
-      <c r="H45">
+      <c r="K45">
         <v>0.63467596745609201</v>
       </c>
-      <c r="I45">
+      <c r="L45">
+        <v>7.5224999999999902</v>
+      </c>
+      <c r="M45">
         <v>1.57885869567682E-2</v>
       </c>
-      <c r="J45">
+      <c r="N45">
         <v>1.4845513997626101</v>
       </c>
-      <c r="K45">
-        <v>7.5224999999999902</v>
-      </c>
-      <c r="L45">
+      <c r="O45">
+        <v>-1.4687628128058401</v>
+      </c>
+      <c r="P45">
+        <v>445.4</v>
+      </c>
+      <c r="Q45">
+        <v>1454.2</v>
+      </c>
+      <c r="R45">
         <v>33.3333333333333</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>40</v>
       </c>
@@ -2871,34 +3731,52 @@
         <v>0.852502746727969</v>
       </c>
       <c r="D46">
+        <v>0.89999999999999902</v>
+      </c>
+      <c r="E46">
         <v>1.85148669498825E-2</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>0.108971434279972</v>
       </c>
-      <c r="F46">
-        <v>0.89999999999999902</v>
-      </c>
       <c r="G46">
+        <v>-9.0456567330089901E-2</v>
+      </c>
+      <c r="H46">
+        <v>160.444444444444</v>
+      </c>
+      <c r="I46">
+        <v>1324.44444444444</v>
+      </c>
+      <c r="J46">
         <v>46</v>
       </c>
-      <c r="H46">
+      <c r="K46">
         <v>0.70179533348967005</v>
       </c>
-      <c r="I46">
+      <c r="L46">
+        <v>6.27666666666663</v>
+      </c>
+      <c r="M46">
         <v>1.7626451637868301E-2</v>
       </c>
-      <c r="J46">
+      <c r="N46">
         <v>0.147107106959494</v>
       </c>
-      <c r="K46">
-        <v>6.27666666666663</v>
-      </c>
-      <c r="L46">
+      <c r="O46">
+        <v>-0.129480655321625</v>
+      </c>
+      <c r="P46">
+        <v>280.444444444444</v>
+      </c>
+      <c r="Q46">
+        <v>1455.55555555555</v>
+      </c>
+      <c r="R46">
         <v>23.9130434782608</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>40</v>
       </c>
@@ -2909,34 +3787,52 @@
         <v>0.75477296131347005</v>
       </c>
       <c r="D47">
+        <v>5.3522727272727</v>
+      </c>
+      <c r="E47">
         <v>1.5674846567855599E-2</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>1.10858020431552</v>
       </c>
-      <c r="F47">
-        <v>5.3522727272727</v>
-      </c>
       <c r="G47">
+        <v>-1.09290535774766</v>
+      </c>
+      <c r="H47">
+        <v>173.72727272727201</v>
+      </c>
+      <c r="I47">
+        <v>1503.6363636363601</v>
+      </c>
+      <c r="J47">
         <v>46</v>
       </c>
-      <c r="H47">
+      <c r="K47">
         <v>0.57774077760676501</v>
       </c>
-      <c r="I47">
+      <c r="L47">
+        <v>9.0804545454545096</v>
+      </c>
+      <c r="M47">
         <v>1.4433370912263E-2</v>
       </c>
-      <c r="J47">
+      <c r="N47">
         <v>0.18936119125686701</v>
       </c>
-      <c r="K47">
-        <v>9.0804545454545096</v>
-      </c>
-      <c r="L47">
+      <c r="O47">
+        <v>-0.174927820344604</v>
+      </c>
+      <c r="P47">
+        <v>539.63636363636294</v>
+      </c>
+      <c r="Q47">
+        <v>1518.6363636363601</v>
+      </c>
+      <c r="R47">
         <v>32.6086956521739</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>40</v>
       </c>
@@ -2947,34 +3843,52 @@
         <v>0.68627192570365403</v>
       </c>
       <c r="D48">
+        <v>7.8374999999999897</v>
+      </c>
+      <c r="E48">
         <v>1.8671071254517401E-2</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>0.24224831405495301</v>
       </c>
-      <c r="F48">
-        <v>7.8374999999999897</v>
-      </c>
       <c r="G48">
+        <v>-0.223577242800436</v>
+      </c>
+      <c r="H48">
+        <v>194.333333333333</v>
+      </c>
+      <c r="I48">
+        <v>1585.4166666666599</v>
+      </c>
+      <c r="J48">
         <v>46</v>
       </c>
-      <c r="H48">
+      <c r="K48">
         <v>0.52428992141344</v>
       </c>
-      <c r="I48">
+      <c r="L48">
+        <v>10.55875</v>
+      </c>
+      <c r="M48">
         <v>1.4006761150321199E-2</v>
       </c>
-      <c r="J48">
+      <c r="N48">
         <v>0.114276791150925</v>
       </c>
-      <c r="K48">
-        <v>10.55875</v>
-      </c>
-      <c r="L48">
+      <c r="O48">
+        <v>-0.100270030000603</v>
+      </c>
+      <c r="P48">
+        <v>591.5</v>
+      </c>
+      <c r="Q48">
+        <v>1558.8333333333301</v>
+      </c>
+      <c r="R48">
         <v>32.6086956521739</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>40</v>
       </c>
@@ -2985,34 +3899,52 @@
         <v>0.69509380912258001</v>
       </c>
       <c r="D49">
+        <v>7.8662499999999502</v>
+      </c>
+      <c r="E49">
         <v>1.8360106465099502E-2</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>0.25330041563538802</v>
       </c>
-      <c r="F49">
-        <v>7.8662499999999502</v>
-      </c>
       <c r="G49">
+        <v>-0.23494030917028899</v>
+      </c>
+      <c r="H49">
+        <v>165</v>
+      </c>
+      <c r="I49">
+        <v>1550.4166666666599</v>
+      </c>
+      <c r="J49">
         <v>46</v>
       </c>
-      <c r="H49">
+      <c r="K49">
         <v>0.52519555272657503</v>
       </c>
-      <c r="I49">
+      <c r="L49">
+        <v>10.098750000000001</v>
+      </c>
+      <c r="M49">
         <v>1.3711341260610899E-2</v>
       </c>
-      <c r="J49">
+      <c r="N49">
         <v>0.10873215039975299</v>
       </c>
-      <c r="K49">
-        <v>10.098750000000001</v>
-      </c>
-      <c r="L49">
+      <c r="O49">
+        <v>-9.5020809139142098E-2</v>
+      </c>
+      <c r="P49">
+        <v>675.66666666666595</v>
+      </c>
+      <c r="Q49">
+        <v>1507.5833333333301</v>
+      </c>
+      <c r="R49">
         <v>32.6086956521739</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>40</v>
       </c>
@@ -3023,34 +3955,52 @@
         <v>0.80640279994758601</v>
       </c>
       <c r="D50">
+        <v>2.7825000000000002</v>
+      </c>
+      <c r="E50">
         <v>1.5141070132590599E-2</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>0.14945414965982901</v>
       </c>
-      <c r="F50">
-        <v>2.7825000000000002</v>
-      </c>
       <c r="G50">
+        <v>-0.13431307952723801</v>
+      </c>
+      <c r="H50">
+        <v>180.7</v>
+      </c>
+      <c r="I50">
+        <v>1425.3</v>
+      </c>
+      <c r="J50">
         <v>45</v>
       </c>
-      <c r="H50">
+      <c r="K50">
         <v>0.63058939910655698</v>
       </c>
-      <c r="I50">
+      <c r="L50">
+        <v>8.2109999999999399</v>
+      </c>
+      <c r="M50">
         <v>1.47473370926617E-2</v>
       </c>
-      <c r="J50">
+      <c r="N50">
         <v>0.126274948537653</v>
       </c>
-      <c r="K50">
-        <v>8.2109999999999399</v>
-      </c>
-      <c r="L50">
+      <c r="O50">
+        <v>-0.111527611444992</v>
+      </c>
+      <c r="P50">
+        <v>383.6</v>
+      </c>
+      <c r="Q50">
+        <v>1533.3</v>
+      </c>
+      <c r="R50">
         <v>31.1111111111111</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>40</v>
       </c>
@@ -3061,34 +4011,52 @@
         <v>0.74810069815687796</v>
       </c>
       <c r="D51">
+        <v>5.10818181818179</v>
+      </c>
+      <c r="E51">
         <v>1.9337920596732401E-2</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>0.18199858092346599</v>
       </c>
-      <c r="F51">
-        <v>5.10818181818179</v>
-      </c>
       <c r="G51">
+        <v>-0.16266066032673299</v>
+      </c>
+      <c r="H51">
+        <v>210.45454545454501</v>
+      </c>
+      <c r="I51">
+        <v>1491.72727272727</v>
+      </c>
+      <c r="J51">
         <v>46</v>
       </c>
-      <c r="H51">
+      <c r="K51">
         <v>0.58175378433678404</v>
       </c>
-      <c r="I51">
+      <c r="L51">
+        <v>8.9345454545454199</v>
+      </c>
+      <c r="M51">
         <v>1.42070852637536E-2</v>
       </c>
-      <c r="J51">
+      <c r="N51">
         <v>0.115241555025749</v>
       </c>
-      <c r="K51">
-        <v>8.9345454545454199</v>
-      </c>
-      <c r="L51">
+      <c r="O51">
+        <v>-0.101034469761996</v>
+      </c>
+      <c r="P51">
+        <v>524.54545454545405</v>
+      </c>
+      <c r="Q51">
+        <v>1524.54545454545</v>
+      </c>
+      <c r="R51">
         <v>32.6086956521739</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B52">
         <f>SUM(B2:B51)</f>
         <v>3004</v>
@@ -3098,39 +4066,63 @@
         <v>0.75437994234678896</v>
       </c>
       <c r="D52">
-        <f t="shared" ref="D52:E52" si="1">SUM(D2:D51)/COUNT(D2:D51)</f>
+        <f t="shared" ref="D52:E52" si="0">SUM(D2:D51)/COUNT(D2:D51)</f>
+        <v>4.9310199883449695</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="0"/>
         <v>1.9663948276889193E-2</v>
-      </c>
-      <c r="E52">
-        <f t="shared" si="1"/>
-        <v>0.26652864826233214</v>
       </c>
       <c r="F52">
         <f>SUM(F2:F51)/COUNT(F2:F51)</f>
-        <v>4.9310199883449695</v>
+        <v>0.26652864826233214</v>
       </c>
       <c r="G52">
-        <f t="shared" ref="G52" si="2">SUM(G2:G51)</f>
-        <v>2305</v>
+        <f>SUM(G2:G51)/COUNT(G2:G51)</f>
+        <v>-0.24686469998544289</v>
       </c>
       <c r="H52">
         <f>SUM(H2:H51)/COUNT(H2:H51)</f>
+        <v>195.21977544677506</v>
+      </c>
+      <c r="I52">
+        <f t="shared" ref="I52:Q52" si="1">SUM(I2:I51)/COUNT(I2:I51)</f>
+        <v>1463.2749704739663</v>
+      </c>
+      <c r="J52">
+        <f>SUM(J2:J51)</f>
+        <v>2305</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="1"/>
         <v>0.58828403089339754</v>
       </c>
-      <c r="I52">
-        <f t="shared" ref="I52:K52" si="3">SUM(I2:I51)/COUNT(I2:I51)</f>
+      <c r="L52">
+        <f t="shared" si="1"/>
+        <v>8.7865401981351745</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="1"/>
         <v>1.4981833987919729E-2</v>
       </c>
-      <c r="J52">
-        <f t="shared" si="3"/>
+      <c r="N52">
+        <f t="shared" si="1"/>
         <v>0.15050920535299253</v>
       </c>
-      <c r="K52">
-        <f t="shared" si="3"/>
-        <v>8.7865401981351745</v>
-      </c>
-      <c r="L52" s="5">
-        <f>(B52-G52)/G52</f>
+      <c r="O52">
+        <f t="shared" si="1"/>
+        <v>-0.1355273713650729</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="1"/>
+        <v>515.77030536130519</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="1"/>
+        <v>1497.5419487179449</v>
+      </c>
+      <c r="R52" s="5">
+        <f>(B52-J52)/J52</f>
         <v>0.30325379609544467</v>
       </c>
     </row>

</xml_diff>